<commit_message>
modificacion .gitignore 08.10 1:53
</commit_message>
<xml_diff>
--- a/flask/app/static/files/exportaciones/historial_solicitudes.xlsx
+++ b/flask/app/static/files/exportaciones/historial_solicitudes.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q79"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -951,7 +951,7 @@
         <v>244</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
@@ -960,7 +960,7 @@
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>123 123</t>
+          <t>Nicolás Felipe Opazo Gana</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
@@ -998,7 +998,7 @@
         <v>244</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>123 123</t>
+          <t>Nicolás Felipe Opazo Gana</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
@@ -1562,29 +1562,29 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>611</v>
+        <v>622</v>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G22" s="2" t="inlineStr">
@@ -1593,16 +1593,16 @@
         </is>
       </c>
       <c r="H22" s="3" t="n">
-        <v>44104.53206018519</v>
+        <v>44105.06001157407</v>
       </c>
       <c r="I22" s="3" t="n">
-        <v>44104.55636574074</v>
+        <v>44105.06001157407</v>
       </c>
       <c r="J22" s="3" t="n">
-        <v>44104.77083333334</v>
+        <v>44110.77083333334</v>
       </c>
       <c r="K22" s="3" t="n">
-        <v>44104.78267361111</v>
+        <v>44110.99744212963</v>
       </c>
       <c r="L22" s="2" t="n"/>
       <c r="M22" s="2" t="n"/>
@@ -1615,10 +1615,10 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
@@ -1632,12 +1632,12 @@
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F23" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G23" s="2" t="inlineStr">
@@ -1646,16 +1646,16 @@
         </is>
       </c>
       <c r="H23" s="3" t="n">
-        <v>44104.07725694445</v>
+        <v>44104.53206018519</v>
       </c>
       <c r="I23" s="3" t="n">
-        <v>44104.49207175926</v>
+        <v>44104.55636574074</v>
       </c>
       <c r="J23" s="3" t="n">
-        <v>44106.77083333334</v>
+        <v>44104.77083333334</v>
       </c>
       <c r="K23" s="3" t="n">
-        <v>44105.03828703704</v>
+        <v>44104.78267361111</v>
       </c>
       <c r="L23" s="2" t="n"/>
       <c r="M23" s="2" t="n"/>
@@ -1668,19 +1668,19 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
@@ -1699,16 +1699,16 @@
         </is>
       </c>
       <c r="H24" s="3" t="n">
-        <v>44104.06814814815</v>
+        <v>44104.07725694445</v>
       </c>
       <c r="I24" s="3" t="n">
-        <v>44104.07643518518</v>
+        <v>44104.49207175926</v>
       </c>
       <c r="J24" s="3" t="n">
-        <v>44116.77083333334</v>
+        <v>44106.77083333334</v>
       </c>
       <c r="K24" s="3" t="n">
-        <v>44108.02783564815</v>
+        <v>44105.03828703704</v>
       </c>
       <c r="L24" s="2" t="n"/>
       <c r="M24" s="2" t="n"/>
@@ -1721,10 +1721,10 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
@@ -1738,12 +1738,12 @@
       </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F25" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G25" s="2" t="inlineStr">
@@ -1752,16 +1752,16 @@
         </is>
       </c>
       <c r="H25" s="3" t="n">
-        <v>44103.99357638889</v>
+        <v>44104.06814814815</v>
       </c>
       <c r="I25" s="3" t="n">
-        <v>44103.99490740741</v>
+        <v>44104.07643518518</v>
       </c>
       <c r="J25" s="3" t="n">
-        <v>44103.77083333334</v>
+        <v>44116.77083333334</v>
       </c>
       <c r="K25" s="3" t="n">
-        <v>44104.003125</v>
+        <v>44108.02783564815</v>
       </c>
       <c r="L25" s="2" t="n"/>
       <c r="M25" s="2" t="n"/>
@@ -1774,57 +1774,55 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H26" s="3" t="n">
-        <v>44103.99023148148</v>
-      </c>
-      <c r="I26" s="2" t="n"/>
-      <c r="J26" s="2" t="n"/>
-      <c r="K26" s="2" t="n"/>
-      <c r="L26" s="3" t="n">
+        <v>44103.99357638889</v>
+      </c>
+      <c r="I26" s="3" t="n">
+        <v>44103.99490740741</v>
+      </c>
+      <c r="J26" s="3" t="n">
         <v>44103.77083333334</v>
       </c>
+      <c r="K26" s="3" t="n">
+        <v>44104.003125</v>
+      </c>
+      <c r="L26" s="2" t="n"/>
       <c r="M26" s="2" t="n"/>
-      <c r="N26" s="3" t="n">
-        <v>44104.06228009259</v>
-      </c>
+      <c r="N26" s="2" t="n"/>
       <c r="O26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P26" s="2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
+      <c r="P26" s="2" t="n"/>
       <c r="Q26" s="2" t="n"/>
     </row>
     <row r="27">
@@ -1832,7 +1830,7 @@
         <v>201</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
@@ -1846,65 +1844,67 @@
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F27" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H27" s="3" t="n">
         <v>44103.99023148148</v>
       </c>
-      <c r="I27" s="3" t="n">
-        <v>44103.9909837963</v>
-      </c>
-      <c r="J27" s="3" t="n">
+      <c r="I27" s="2" t="n"/>
+      <c r="J27" s="2" t="n"/>
+      <c r="K27" s="2" t="n"/>
+      <c r="L27" s="3" t="n">
         <v>44103.77083333334</v>
       </c>
-      <c r="K27" s="3" t="n">
-        <v>44104.55571759259</v>
-      </c>
-      <c r="L27" s="2" t="n"/>
       <c r="M27" s="2" t="n"/>
-      <c r="N27" s="2" t="n"/>
+      <c r="N27" s="3" t="n">
+        <v>44104.06228009259</v>
+      </c>
       <c r="O27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P27" s="2" t="n"/>
+      <c r="P27" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
       <c r="Q27" s="2" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>583</v>
+        <v>599</v>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G28" s="2" t="inlineStr">
@@ -1913,16 +1913,16 @@
         </is>
       </c>
       <c r="H28" s="3" t="n">
-        <v>44100.91527777778</v>
+        <v>44103.99023148148</v>
       </c>
       <c r="I28" s="3" t="n">
-        <v>44103.82704861111</v>
+        <v>44103.9909837963</v>
       </c>
       <c r="J28" s="3" t="n">
-        <v>44106.77083333334</v>
+        <v>44103.77083333334</v>
       </c>
       <c r="K28" s="3" t="n">
-        <v>44103.84380787037</v>
+        <v>44104.55571759259</v>
       </c>
       <c r="L28" s="2" t="n"/>
       <c r="M28" s="2" t="n"/>
@@ -1935,10 +1935,10 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
@@ -1952,12 +1952,12 @@
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G29" s="2" t="inlineStr">
@@ -1966,16 +1966,16 @@
         </is>
       </c>
       <c r="H29" s="3" t="n">
-        <v>44100.04094907407</v>
+        <v>44100.91527777778</v>
       </c>
       <c r="I29" s="3" t="n">
-        <v>44100.04094907407</v>
+        <v>44103.82704861111</v>
       </c>
       <c r="J29" s="3" t="n">
-        <v>44102.77083333334</v>
+        <v>44106.77083333334</v>
       </c>
       <c r="K29" s="3" t="n">
-        <v>44100.90773148148</v>
+        <v>44103.84380787037</v>
       </c>
       <c r="L29" s="2" t="n"/>
       <c r="M29" s="2" t="n"/>
@@ -1991,7 +1991,7 @@
         <v>193</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
@@ -2005,12 +2005,12 @@
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G30" s="2" t="inlineStr">
@@ -2028,7 +2028,7 @@
         <v>44102.77083333334</v>
       </c>
       <c r="K30" s="3" t="n">
-        <v>44102.02782407407</v>
+        <v>44100.90773148148</v>
       </c>
       <c r="L30" s="2" t="n"/>
       <c r="M30" s="2" t="n"/>
@@ -2041,19 +2041,19 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E31" s="2" t="inlineStr">
@@ -2072,16 +2072,16 @@
         </is>
       </c>
       <c r="H31" s="3" t="n">
-        <v>44100.03137731482</v>
+        <v>44100.04094907407</v>
       </c>
       <c r="I31" s="3" t="n">
-        <v>44100.03137731482</v>
+        <v>44100.04094907407</v>
       </c>
       <c r="J31" s="3" t="n">
-        <v>44104.77083333334</v>
+        <v>44102.77083333334</v>
       </c>
       <c r="K31" s="3" t="n">
-        <v>44103.90252314815</v>
+        <v>44102.02782407407</v>
       </c>
       <c r="L31" s="2" t="n"/>
       <c r="M31" s="2" t="n"/>
@@ -2094,10 +2094,10 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
@@ -2111,12 +2111,12 @@
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G32" s="2" t="inlineStr">
@@ -2125,16 +2125,16 @@
         </is>
       </c>
       <c r="H32" s="3" t="n">
-        <v>44099.99474537037</v>
+        <v>44100.03137731482</v>
       </c>
       <c r="I32" s="3" t="n">
-        <v>44099.99474537037</v>
+        <v>44100.03137731482</v>
       </c>
       <c r="J32" s="3" t="n">
-        <v>44102.77083333334</v>
+        <v>44104.77083333334</v>
       </c>
       <c r="K32" s="3" t="n">
-        <v>44102.02828703704</v>
+        <v>44103.90252314815</v>
       </c>
       <c r="L32" s="2" t="n"/>
       <c r="M32" s="2" t="n"/>
@@ -2147,10 +2147,10 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>554</v>
+        <v>572</v>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
@@ -2164,12 +2164,12 @@
       </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F33" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G33" s="2" t="inlineStr">
@@ -2178,32 +2178,32 @@
         </is>
       </c>
       <c r="H33" s="3" t="n">
-        <v>44099.56803240741</v>
+        <v>44099.99474537037</v>
       </c>
       <c r="I33" s="3" t="n">
-        <v>44099.6490162037</v>
+        <v>44099.99474537037</v>
       </c>
       <c r="J33" s="3" t="n">
-        <v>44109.77083333334</v>
+        <v>44102.77083333334</v>
       </c>
       <c r="K33" s="3" t="n">
-        <v>44103.90502314815</v>
+        <v>44102.02828703704</v>
       </c>
       <c r="L33" s="2" t="n"/>
       <c r="M33" s="2" t="n"/>
       <c r="N33" s="2" t="n"/>
       <c r="O33" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P33" s="2" t="n"/>
       <c r="Q33" s="2" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>508</v>
+        <v>554</v>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
@@ -2227,29 +2227,28 @@
       </c>
       <c r="G34" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H34" s="3" t="n">
-        <v>44094.73216435185</v>
-      </c>
-      <c r="I34" s="2" t="n"/>
-      <c r="J34" s="2" t="n"/>
-      <c r="K34" s="2" t="n"/>
+        <v>44099.56803240741</v>
+      </c>
+      <c r="I34" s="3" t="n">
+        <v>44099.6490162037</v>
+      </c>
+      <c r="J34" s="3" t="n">
+        <v>44109.77083333334</v>
+      </c>
+      <c r="K34" s="3" t="n">
+        <v>44103.90502314815</v>
+      </c>
       <c r="L34" s="2" t="n"/>
-      <c r="M34" s="3" t="n">
-        <v>44094.75707175926</v>
-      </c>
+      <c r="M34" s="2" t="n"/>
       <c r="N34" s="2" t="n"/>
       <c r="O34" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P34" s="2" t="inlineStr">
-        <is>
-          <t>Prueba de rechazo de solicitud
-LabEIT.-</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="P34" s="2" t="n"/>
       <c r="Q34" s="2" t="n"/>
     </row>
     <row r="35">
@@ -2257,7 +2256,7 @@
         <v>154</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
@@ -2271,17 +2270,17 @@
       </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F35" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G35" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H35" s="3" t="n">
@@ -2290,139 +2289,140 @@
       <c r="I35" s="2" t="n"/>
       <c r="J35" s="2" t="n"/>
       <c r="K35" s="2" t="n"/>
-      <c r="L35" s="3" t="n">
+      <c r="L35" s="2" t="n"/>
+      <c r="M35" s="3" t="n">
+        <v>44094.75707175926</v>
+      </c>
+      <c r="N35" s="2" t="n"/>
+      <c r="O35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" s="2" t="inlineStr">
+        <is>
+          <t>Prueba de rechazo de solicitud
+LabEIT.-</t>
+        </is>
+      </c>
+      <c r="Q35" s="2" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>154</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>510</v>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>19889608K</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>Sebastián Ignacio Toro Severino</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>Router TP-LINK TL-WN722N</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>AAA351</t>
+        </is>
+      </c>
+      <c r="G36" s="2" t="inlineStr">
+        <is>
+          <t>Cancelada</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>44094.73216435185</v>
+      </c>
+      <c r="I36" s="2" t="n"/>
+      <c r="J36" s="2" t="n"/>
+      <c r="K36" s="2" t="n"/>
+      <c r="L36" s="3" t="n">
         <v>44096.77083333334</v>
       </c>
-      <c r="M35" s="2" t="n"/>
-      <c r="N35" s="3" t="n">
+      <c r="M36" s="2" t="n"/>
+      <c r="N36" s="3" t="n">
         <v>44094.73256944444</v>
       </c>
-      <c r="O35" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P35" s="2" t="inlineStr">
+      <c r="O36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" s="2" t="inlineStr">
         <is>
           <t>Cancelación de prueba
 LabEIT
 2020</t>
         </is>
       </c>
-      <c r="Q35" s="2" t="n"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
+      <c r="Q36" s="2" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
         <v>154</v>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B37" s="2" t="n">
         <v>511</v>
       </c>
-      <c r="C36" s="2" t="inlineStr">
+      <c r="C37" s="2" t="inlineStr">
         <is>
           <t>19889608K</t>
         </is>
       </c>
-      <c r="D36" s="2" t="inlineStr">
+      <c r="D37" s="2" t="inlineStr">
         <is>
           <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
-      <c r="E36" s="2" t="inlineStr">
+      <c r="E37" s="2" t="inlineStr">
         <is>
           <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
-      <c r="F36" s="2" t="inlineStr">
+      <c r="F37" s="2" t="inlineStr">
         <is>
           <t>AAA351</t>
         </is>
       </c>
-      <c r="G36" s="2" t="inlineStr">
+      <c r="G37" s="2" t="inlineStr">
         <is>
           <t>Rechazada</t>
         </is>
       </c>
-      <c r="H36" s="3" t="n">
+      <c r="H37" s="3" t="n">
         <v>44094.73216435185</v>
       </c>
-      <c r="I36" s="2" t="n"/>
-      <c r="J36" s="2" t="n"/>
-      <c r="K36" s="2" t="n"/>
-      <c r="L36" s="2" t="n"/>
-      <c r="M36" s="3" t="n">
+      <c r="I37" s="2" t="n"/>
+      <c r="J37" s="2" t="n"/>
+      <c r="K37" s="2" t="n"/>
+      <c r="L37" s="2" t="n"/>
+      <c r="M37" s="3" t="n">
         <v>44094.73327546296</v>
       </c>
-      <c r="N36" s="2" t="n"/>
-      <c r="O36" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P36" s="2" t="inlineStr">
+      <c r="N37" s="2" t="n"/>
+      <c r="O37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2" t="inlineStr">
         <is>
           <t>Prueba de rechazo
 LabEIT
 2020</t>
         </is>
       </c>
-      <c r="Q36" s="2" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
-        <v>87</v>
-      </c>
-      <c r="B37" s="2" t="n">
-        <v>294</v>
-      </c>
-      <c r="C37" s="2" t="inlineStr">
-        <is>
-          <t>19988806K</t>
-        </is>
-      </c>
-      <c r="D37" s="2" t="inlineStr">
-        <is>
-          <t>Sebastián Toro</t>
-        </is>
-      </c>
-      <c r="E37" s="2" t="inlineStr">
-        <is>
-          <t>Notebook  Asus 636-512</t>
-        </is>
-      </c>
-      <c r="F37" s="2" t="inlineStr">
-        <is>
-          <t>ZZZZZ6</t>
-        </is>
-      </c>
-      <c r="G37" s="2" t="inlineStr">
-        <is>
-          <t>Finalizada</t>
-        </is>
-      </c>
-      <c r="H37" s="3" t="n">
-        <v>44068.93978009259</v>
-      </c>
-      <c r="I37" s="3" t="n">
-        <v>44068.98197916667</v>
-      </c>
-      <c r="J37" s="3" t="n">
-        <v>44068.77083333334</v>
-      </c>
-      <c r="K37" s="3" t="n">
-        <v>44068.98927083334</v>
-      </c>
-      <c r="L37" s="2" t="n"/>
-      <c r="M37" s="2" t="n"/>
-      <c r="N37" s="2" t="n"/>
-      <c r="O37" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" s="2" t="n"/>
       <c r="Q37" s="2" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
@@ -2436,12 +2436,12 @@
       </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G38" s="2" t="inlineStr">
@@ -2450,16 +2450,16 @@
         </is>
       </c>
       <c r="H38" s="3" t="n">
-        <v>44068.903125</v>
+        <v>44068.93978009259</v>
       </c>
       <c r="I38" s="3" t="n">
-        <v>44068.98976851852</v>
+        <v>44068.98197916667</v>
       </c>
       <c r="J38" s="3" t="n">
         <v>44068.77083333334</v>
       </c>
       <c r="K38" s="3" t="n">
-        <v>44068.99473379629</v>
+        <v>44068.98927083334</v>
       </c>
       <c r="L38" s="2" t="n"/>
       <c r="M38" s="2" t="n"/>
@@ -2472,10 +2472,10 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
@@ -2489,12 +2489,12 @@
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F39" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G39" s="2" t="inlineStr">
@@ -2503,16 +2503,16 @@
         </is>
       </c>
       <c r="H39" s="3" t="n">
-        <v>44068.63998842592</v>
+        <v>44068.903125</v>
       </c>
       <c r="I39" s="3" t="n">
-        <v>44068.94631944445</v>
+        <v>44068.98976851852</v>
       </c>
       <c r="J39" s="3" t="n">
-        <v>44081.77083333334</v>
+        <v>44068.77083333334</v>
       </c>
       <c r="K39" s="3" t="n">
-        <v>44072.94930555556</v>
+        <v>44068.99473379629</v>
       </c>
       <c r="L39" s="2" t="n"/>
       <c r="M39" s="2" t="n"/>
@@ -2525,10 +2525,10 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
@@ -2542,32 +2542,34 @@
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H40" s="3" t="n">
-        <v>44067.97563657408</v>
-      </c>
-      <c r="I40" s="2" t="n"/>
-      <c r="J40" s="2" t="n"/>
-      <c r="K40" s="2" t="n"/>
-      <c r="L40" s="3" t="n">
-        <v>44069.77083333334</v>
-      </c>
+        <v>44068.63998842592</v>
+      </c>
+      <c r="I40" s="3" t="n">
+        <v>44068.94631944445</v>
+      </c>
+      <c r="J40" s="3" t="n">
+        <v>44081.77083333334</v>
+      </c>
+      <c r="K40" s="3" t="n">
+        <v>44072.94930555556</v>
+      </c>
+      <c r="L40" s="2" t="n"/>
       <c r="M40" s="2" t="n"/>
-      <c r="N40" s="3" t="n">
-        <v>44068.02151620371</v>
-      </c>
+      <c r="N40" s="2" t="n"/>
       <c r="O40" s="2" t="n">
         <v>0</v>
       </c>
@@ -2576,10 +2578,10 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
@@ -2593,30 +2595,32 @@
       </c>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G41" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H41" s="3" t="n">
-        <v>44067.97258101852</v>
+        <v>44067.97563657408</v>
       </c>
       <c r="I41" s="2" t="n"/>
       <c r="J41" s="2" t="n"/>
       <c r="K41" s="2" t="n"/>
-      <c r="L41" s="2" t="n"/>
-      <c r="M41" s="3" t="n">
-        <v>44068.01609953704</v>
-      </c>
-      <c r="N41" s="2" t="n"/>
+      <c r="L41" s="3" t="n">
+        <v>44069.77083333334</v>
+      </c>
+      <c r="M41" s="2" t="n"/>
+      <c r="N41" s="3" t="n">
+        <v>44068.02151620371</v>
+      </c>
       <c r="O41" s="2" t="n">
         <v>0</v>
       </c>
@@ -2628,7 +2632,7 @@
         <v>83</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
@@ -2642,12 +2646,12 @@
       </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G42" s="2" t="inlineStr">
@@ -2663,7 +2667,7 @@
       <c r="K42" s="2" t="n"/>
       <c r="L42" s="2" t="n"/>
       <c r="M42" s="3" t="n">
-        <v>44068.01634259259</v>
+        <v>44068.01609953704</v>
       </c>
       <c r="N42" s="2" t="n"/>
       <c r="O42" s="2" t="n">
@@ -2674,10 +2678,10 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
@@ -2691,36 +2695,32 @@
       </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G43" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H43" s="3" t="n">
-        <v>44067.96421296296</v>
-      </c>
-      <c r="I43" s="3" t="n">
-        <v>44068.00895833333</v>
-      </c>
-      <c r="J43" s="3" t="n">
-        <v>44075.77083333334</v>
-      </c>
-      <c r="K43" s="3" t="n">
-        <v>44068.93479166667</v>
-      </c>
+        <v>44067.97258101852</v>
+      </c>
+      <c r="I43" s="2" t="n"/>
+      <c r="J43" s="2" t="n"/>
+      <c r="K43" s="2" t="n"/>
       <c r="L43" s="2" t="n"/>
-      <c r="M43" s="2" t="n"/>
+      <c r="M43" s="3" t="n">
+        <v>44068.01634259259</v>
+      </c>
       <c r="N43" s="2" t="n"/>
       <c r="O43" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P43" s="2" t="n"/>
       <c r="Q43" s="2" t="n"/>
@@ -2730,7 +2730,7 @@
         <v>82</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
@@ -2744,12 +2744,12 @@
       </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G44" s="2" t="inlineStr">
@@ -2761,29 +2761,29 @@
         <v>44067.96421296296</v>
       </c>
       <c r="I44" s="3" t="n">
-        <v>44068.99569444444</v>
+        <v>44068.00895833333</v>
       </c>
       <c r="J44" s="3" t="n">
-        <v>44068.77083333334</v>
+        <v>44075.77083333334</v>
       </c>
       <c r="K44" s="3" t="n">
-        <v>44068.99739583334</v>
+        <v>44068.93479166667</v>
       </c>
       <c r="L44" s="2" t="n"/>
       <c r="M44" s="2" t="n"/>
       <c r="N44" s="2" t="n"/>
       <c r="O44" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P44" s="2" t="n"/>
       <c r="Q44" s="2" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
@@ -2797,29 +2797,33 @@
       </c>
       <c r="E45" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G45" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H45" s="3" t="n">
-        <v>44066.73674768519</v>
-      </c>
-      <c r="I45" s="2" t="n"/>
-      <c r="J45" s="2" t="n"/>
-      <c r="K45" s="2" t="n"/>
+        <v>44067.96421296296</v>
+      </c>
+      <c r="I45" s="3" t="n">
+        <v>44068.99569444444</v>
+      </c>
+      <c r="J45" s="3" t="n">
+        <v>44068.77083333334</v>
+      </c>
+      <c r="K45" s="3" t="n">
+        <v>44068.99739583334</v>
+      </c>
       <c r="L45" s="2" t="n"/>
-      <c r="M45" s="3" t="n">
-        <v>44066.78075231481</v>
-      </c>
+      <c r="M45" s="2" t="n"/>
       <c r="N45" s="2" t="n"/>
       <c r="O45" s="2" t="n">
         <v>0</v>
@@ -2832,7 +2836,7 @@
         <v>79</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
@@ -2856,23 +2860,19 @@
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H46" s="3" t="n">
         <v>44066.73674768519</v>
       </c>
-      <c r="I46" s="3" t="n">
-        <v>44069</v>
-      </c>
-      <c r="J46" s="3" t="n">
-        <v>44069.77083333334</v>
-      </c>
-      <c r="K46" s="3" t="n">
-        <v>44069.00579861111</v>
-      </c>
+      <c r="I46" s="2" t="n"/>
+      <c r="J46" s="2" t="n"/>
+      <c r="K46" s="2" t="n"/>
       <c r="L46" s="2" t="n"/>
-      <c r="M46" s="2" t="n"/>
+      <c r="M46" s="3" t="n">
+        <v>44066.78075231481</v>
+      </c>
       <c r="N46" s="2" t="n"/>
       <c r="O46" s="2" t="n">
         <v>0</v>
@@ -2885,7 +2885,7 @@
         <v>79</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
@@ -2916,13 +2916,13 @@
         <v>44066.73674768519</v>
       </c>
       <c r="I47" s="3" t="n">
-        <v>44068.00912037037</v>
+        <v>44069</v>
       </c>
       <c r="J47" s="3" t="n">
-        <v>44075.77083333334</v>
+        <v>44069.77083333334</v>
       </c>
       <c r="K47" s="3" t="n">
-        <v>44068.94960648148</v>
+        <v>44069.00579861111</v>
       </c>
       <c r="L47" s="2" t="n"/>
       <c r="M47" s="2" t="n"/>
@@ -2935,10 +2935,10 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
@@ -2952,32 +2952,34 @@
       </c>
       <c r="E48" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G48" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H48" s="3" t="n">
-        <v>44064.54511574074</v>
-      </c>
-      <c r="I48" s="2" t="n"/>
-      <c r="J48" s="2" t="n"/>
-      <c r="K48" s="2" t="n"/>
-      <c r="L48" s="3" t="n">
-        <v>44072.77083333334</v>
-      </c>
+        <v>44066.73674768519</v>
+      </c>
+      <c r="I48" s="3" t="n">
+        <v>44068.00912037037</v>
+      </c>
+      <c r="J48" s="3" t="n">
+        <v>44075.77083333334</v>
+      </c>
+      <c r="K48" s="3" t="n">
+        <v>44068.94960648148</v>
+      </c>
+      <c r="L48" s="2" t="n"/>
       <c r="M48" s="2" t="n"/>
-      <c r="N48" s="3" t="n">
-        <v>44064.58971064815</v>
-      </c>
+      <c r="N48" s="2" t="n"/>
       <c r="O48" s="2" t="n">
         <v>0</v>
       </c>
@@ -2989,7 +2991,7 @@
         <v>77</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
@@ -3013,7 +3015,7 @@
       </c>
       <c r="G49" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H49" s="3" t="n">
@@ -3022,11 +3024,13 @@
       <c r="I49" s="2" t="n"/>
       <c r="J49" s="2" t="n"/>
       <c r="K49" s="2" t="n"/>
-      <c r="L49" s="2" t="n"/>
-      <c r="M49" s="3" t="n">
-        <v>44064.58886574074</v>
-      </c>
-      <c r="N49" s="2" t="n"/>
+      <c r="L49" s="3" t="n">
+        <v>44072.77083333334</v>
+      </c>
+      <c r="M49" s="2" t="n"/>
+      <c r="N49" s="3" t="n">
+        <v>44064.58971064815</v>
+      </c>
       <c r="O49" s="2" t="n">
         <v>0</v>
       </c>
@@ -3035,50 +3039,46 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D50" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E50" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G50" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H50" s="3" t="n">
-        <v>44062.72828703704</v>
-      </c>
-      <c r="I50" s="3" t="n">
-        <v>44063.58475694444</v>
-      </c>
-      <c r="J50" s="3" t="n">
-        <v>44063.77083333334</v>
-      </c>
-      <c r="K50" s="3" t="n">
-        <v>44063.59297453704</v>
-      </c>
+        <v>44064.54511574074</v>
+      </c>
+      <c r="I50" s="2" t="n"/>
+      <c r="J50" s="2" t="n"/>
+      <c r="K50" s="2" t="n"/>
       <c r="L50" s="2" t="n"/>
-      <c r="M50" s="2" t="n"/>
+      <c r="M50" s="3" t="n">
+        <v>44064.58886574074</v>
+      </c>
       <c r="N50" s="2" t="n"/>
       <c r="O50" s="2" t="n">
         <v>0</v>
@@ -3088,19 +3088,19 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E51" s="2" t="inlineStr">
@@ -3119,32 +3119,32 @@
         </is>
       </c>
       <c r="H51" s="3" t="n">
-        <v>44059.52234953704</v>
+        <v>44062.72828703704</v>
       </c>
       <c r="I51" s="3" t="n">
-        <v>44059.5640162037</v>
+        <v>44063.58475694444</v>
       </c>
       <c r="J51" s="3" t="n">
-        <v>44077.77083333334</v>
+        <v>44063.77083333334</v>
       </c>
       <c r="K51" s="3" t="n">
-        <v>44064.57136574074</v>
+        <v>44063.59297453704</v>
       </c>
       <c r="L51" s="2" t="n"/>
       <c r="M51" s="2" t="n"/>
       <c r="N51" s="2" t="n"/>
       <c r="O51" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P51" s="2" t="n"/>
       <c r="Q51" s="2" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
@@ -3158,12 +3158,12 @@
       </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F52" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G52" s="2" t="inlineStr">
@@ -3172,32 +3172,32 @@
         </is>
       </c>
       <c r="H52" s="3" t="n">
-        <v>44059.4880787037</v>
+        <v>44059.52234953704</v>
       </c>
       <c r="I52" s="3" t="n">
-        <v>44059.53171296296</v>
+        <v>44059.5640162037</v>
       </c>
       <c r="J52" s="3" t="n">
-        <v>44071.77083333334</v>
+        <v>44077.77083333334</v>
       </c>
       <c r="K52" s="3" t="n">
-        <v>44070.67811342593</v>
+        <v>44064.57136574074</v>
       </c>
       <c r="L52" s="2" t="n"/>
       <c r="M52" s="2" t="n"/>
       <c r="N52" s="2" t="n"/>
       <c r="O52" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P52" s="2" t="n"/>
       <c r="Q52" s="2" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
@@ -3211,12 +3211,12 @@
       </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F53" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G53" s="2" t="inlineStr">
@@ -3225,16 +3225,16 @@
         </is>
       </c>
       <c r="H53" s="3" t="n">
-        <v>44058.48174768518</v>
+        <v>44059.4880787037</v>
       </c>
       <c r="I53" s="3" t="n">
-        <v>44059.53150462963</v>
+        <v>44059.53171296296</v>
       </c>
       <c r="J53" s="3" t="n">
-        <v>44061.77083333334</v>
+        <v>44071.77083333334</v>
       </c>
       <c r="K53" s="3" t="n">
-        <v>44062.5589699074</v>
+        <v>44070.67811342593</v>
       </c>
       <c r="L53" s="2" t="n"/>
       <c r="M53" s="2" t="n"/>
@@ -3247,19 +3247,19 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D54" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E54" s="2" t="inlineStr">
@@ -3274,18 +3274,22 @@
       </c>
       <c r="G54" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H54" s="3" t="n">
-        <v>44053.7452662037</v>
-      </c>
-      <c r="I54" s="2" t="n"/>
-      <c r="J54" s="2" t="n"/>
-      <c r="K54" s="2" t="n"/>
-      <c r="L54" s="3" t="n">
+        <v>44058.48174768518</v>
+      </c>
+      <c r="I54" s="3" t="n">
+        <v>44059.53150462963</v>
+      </c>
+      <c r="J54" s="3" t="n">
         <v>44061.77083333334</v>
       </c>
+      <c r="K54" s="3" t="n">
+        <v>44062.5589699074</v>
+      </c>
+      <c r="L54" s="2" t="n"/>
       <c r="M54" s="2" t="n"/>
       <c r="N54" s="2" t="n"/>
       <c r="O54" s="2" t="n">
@@ -3296,49 +3300,45 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E55" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F55" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H55" s="3" t="n">
-        <v>44051.60150462963</v>
-      </c>
-      <c r="I55" s="3" t="n">
-        <v>44051.6865625</v>
-      </c>
-      <c r="J55" s="3" t="n">
-        <v>44053.77083333334</v>
-      </c>
-      <c r="K55" s="3" t="n">
-        <v>44053.79626157408</v>
-      </c>
-      <c r="L55" s="2" t="n"/>
+        <v>44053.7452662037</v>
+      </c>
+      <c r="I55" s="2" t="n"/>
+      <c r="J55" s="2" t="n"/>
+      <c r="K55" s="2" t="n"/>
+      <c r="L55" s="3" t="n">
+        <v>44061.77083333334</v>
+      </c>
       <c r="M55" s="2" t="n"/>
       <c r="N55" s="2" t="n"/>
       <c r="O55" s="2" t="n">
@@ -3349,19 +3349,19 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>198182354</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Víctor Esteban Sánchez Ulloa</t>
         </is>
       </c>
       <c r="E56" s="2" t="inlineStr">
@@ -3380,64 +3380,70 @@
         </is>
       </c>
       <c r="H56" s="3" t="n">
-        <v>44050.4183449074</v>
+        <v>44051.89761574074</v>
       </c>
       <c r="I56" s="3" t="n">
-        <v>44051.54168981482</v>
+        <v>44051.94155092593</v>
       </c>
       <c r="J56" s="3" t="n">
-        <v>44051.77083333334</v>
+        <v>44155.77083333334</v>
       </c>
       <c r="K56" s="3" t="n">
-        <v>44051.54444444444</v>
+        <v>44110.99850694444</v>
       </c>
       <c r="L56" s="2" t="n"/>
       <c r="M56" s="2" t="n"/>
       <c r="N56" s="2" t="n"/>
       <c r="O56" s="2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P56" s="2" t="n"/>
       <c r="Q56" s="2" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F57" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H57" s="3" t="n">
-        <v>44050.4183449074</v>
-      </c>
-      <c r="I57" s="2" t="n"/>
-      <c r="J57" s="2" t="n"/>
-      <c r="K57" s="2" t="n"/>
+        <v>44051.60150462963</v>
+      </c>
+      <c r="I57" s="3" t="n">
+        <v>44051.6865625</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>44053.77083333334</v>
+      </c>
+      <c r="K57" s="3" t="n">
+        <v>44053.79626157408</v>
+      </c>
       <c r="L57" s="2" t="n"/>
       <c r="M57" s="2" t="n"/>
       <c r="N57" s="2" t="n"/>
@@ -3452,7 +3458,7 @@
         <v>63</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
@@ -3466,12 +3472,12 @@
       </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G58" s="2" t="inlineStr">
@@ -3496,10 +3502,10 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
@@ -3513,28 +3519,26 @@
       </c>
       <c r="E59" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F59" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G59" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H59" s="3" t="n">
-        <v>44047.52844907407</v>
+        <v>44050.4183449074</v>
       </c>
       <c r="I59" s="2" t="n"/>
       <c r="J59" s="2" t="n"/>
       <c r="K59" s="2" t="n"/>
-      <c r="L59" s="3" t="n">
-        <v>44049.77083333334</v>
-      </c>
+      <c r="L59" s="2" t="n"/>
       <c r="M59" s="2" t="n"/>
       <c r="N59" s="2" t="n"/>
       <c r="O59" s="2" t="n">
@@ -3545,10 +3549,10 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
@@ -3562,25 +3566,31 @@
       </c>
       <c r="E60" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H60" s="3" t="n">
-        <v>44047.49662037037</v>
-      </c>
-      <c r="I60" s="2" t="n"/>
-      <c r="J60" s="2" t="n"/>
-      <c r="K60" s="2" t="n"/>
+        <v>44050.4183449074</v>
+      </c>
+      <c r="I60" s="3" t="n">
+        <v>44051.54168981482</v>
+      </c>
+      <c r="J60" s="3" t="n">
+        <v>44051.77083333334</v>
+      </c>
+      <c r="K60" s="3" t="n">
+        <v>44051.54444444444</v>
+      </c>
       <c r="L60" s="2" t="n"/>
       <c r="M60" s="2" t="n"/>
       <c r="N60" s="2" t="n"/>
@@ -3592,49 +3602,45 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>198182354</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr">
         <is>
-          <t>Víctor Esteban Sánchez Ulloa</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E61" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F61" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G61" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H61" s="3" t="n">
-        <v>44045.12303240741</v>
-      </c>
-      <c r="I61" s="3" t="n">
-        <v>44048.15038194445</v>
-      </c>
-      <c r="J61" s="3" t="n">
-        <v>44060.77083333334</v>
-      </c>
-      <c r="K61" s="3" t="n">
-        <v>44048.15122685185</v>
-      </c>
-      <c r="L61" s="2" t="n"/>
+        <v>44047.52844907407</v>
+      </c>
+      <c r="I61" s="2" t="n"/>
+      <c r="J61" s="2" t="n"/>
+      <c r="K61" s="2" t="n"/>
+      <c r="L61" s="3" t="n">
+        <v>44049.77083333334</v>
+      </c>
       <c r="M61" s="2" t="n"/>
       <c r="N61" s="2" t="n"/>
       <c r="O61" s="2" t="n">
@@ -3645,10 +3651,10 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
@@ -3662,31 +3668,25 @@
       </c>
       <c r="E62" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G62" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H62" s="3" t="n">
-        <v>44044.55893518519</v>
-      </c>
-      <c r="I62" s="3" t="n">
-        <v>44044.60060185185</v>
-      </c>
-      <c r="J62" s="3" t="n">
-        <v>44050.77083333334</v>
-      </c>
-      <c r="K62" s="3" t="n">
-        <v>44050.4495949074</v>
-      </c>
+        <v>44047.49662037037</v>
+      </c>
+      <c r="I62" s="2" t="n"/>
+      <c r="J62" s="2" t="n"/>
+      <c r="K62" s="2" t="n"/>
       <c r="L62" s="2" t="n"/>
       <c r="M62" s="2" t="n"/>
       <c r="N62" s="2" t="n"/>
@@ -3698,29 +3698,29 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>198182354</t>
         </is>
       </c>
       <c r="D63" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Víctor Esteban Sánchez Ulloa</t>
         </is>
       </c>
       <c r="E63" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F63" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G63" s="2" t="inlineStr">
@@ -3729,16 +3729,16 @@
         </is>
       </c>
       <c r="H63" s="3" t="n">
-        <v>44044.53820601852</v>
+        <v>44045.12303240741</v>
       </c>
       <c r="I63" s="3" t="n">
-        <v>44044.57987268519</v>
+        <v>44048.15038194445</v>
       </c>
       <c r="J63" s="3" t="n">
-        <v>44056.77083333334</v>
+        <v>44060.77083333334</v>
       </c>
       <c r="K63" s="3" t="n">
-        <v>44059.50581018518</v>
+        <v>44048.15122685185</v>
       </c>
       <c r="L63" s="2" t="n"/>
       <c r="M63" s="2" t="n"/>
@@ -3751,10 +3751,10 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
@@ -3768,12 +3768,12 @@
       </c>
       <c r="E64" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G64" s="2" t="inlineStr">
@@ -3782,16 +3782,16 @@
         </is>
       </c>
       <c r="H64" s="3" t="n">
-        <v>44044.53820601852</v>
+        <v>44044.55893518519</v>
       </c>
       <c r="I64" s="3" t="n">
-        <v>44044.57987268519</v>
+        <v>44044.60060185185</v>
       </c>
       <c r="J64" s="3" t="n">
-        <v>44048.77083333334</v>
+        <v>44050.77083333334</v>
       </c>
       <c r="K64" s="3" t="n">
-        <v>44049.66491898148</v>
+        <v>44050.4495949074</v>
       </c>
       <c r="L64" s="2" t="n"/>
       <c r="M64" s="2" t="n"/>
@@ -3804,42 +3804,48 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
-          <t>198182354</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D65" s="2" t="inlineStr">
         <is>
-          <t>Víctor Esteban Sánchez Ulloa</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E65" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F65" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G65" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H65" s="3" t="n">
-        <v>44044.10501157407</v>
-      </c>
-      <c r="I65" s="2" t="n"/>
-      <c r="J65" s="2" t="n"/>
-      <c r="K65" s="2" t="n"/>
+        <v>44044.53820601852</v>
+      </c>
+      <c r="I65" s="3" t="n">
+        <v>44044.57987268519</v>
+      </c>
+      <c r="J65" s="3" t="n">
+        <v>44056.77083333334</v>
+      </c>
+      <c r="K65" s="3" t="n">
+        <v>44059.50581018518</v>
+      </c>
       <c r="L65" s="2" t="n"/>
       <c r="M65" s="2" t="n"/>
       <c r="N65" s="2" t="n"/>
@@ -3851,42 +3857,48 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>198182354</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D66" s="2" t="inlineStr">
         <is>
-          <t>Víctor Esteban Sánchez Ulloa</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E66" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G66" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H66" s="3" t="n">
-        <v>44044.10501157407</v>
-      </c>
-      <c r="I66" s="2" t="n"/>
-      <c r="J66" s="2" t="n"/>
-      <c r="K66" s="2" t="n"/>
+        <v>44044.53820601852</v>
+      </c>
+      <c r="I66" s="3" t="n">
+        <v>44044.57987268519</v>
+      </c>
+      <c r="J66" s="3" t="n">
+        <v>44048.77083333334</v>
+      </c>
+      <c r="K66" s="3" t="n">
+        <v>44049.66491898148</v>
+      </c>
       <c r="L66" s="2" t="n"/>
       <c r="M66" s="2" t="n"/>
       <c r="N66" s="2" t="n"/>
@@ -3945,10 +3957,10 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B68" s="2" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
@@ -3962,12 +3974,12 @@
       </c>
       <c r="E68" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G68" s="2" t="inlineStr">
@@ -3976,7 +3988,7 @@
         </is>
       </c>
       <c r="H68" s="3" t="n">
-        <v>44044.09211805555</v>
+        <v>44044.10501157407</v>
       </c>
       <c r="I68" s="2" t="n"/>
       <c r="J68" s="2" t="n"/>
@@ -3992,19 +4004,19 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>198182354</t>
         </is>
       </c>
       <c r="D69" s="2" t="inlineStr">
         <is>
-          <t>Matías Severino</t>
+          <t>Víctor Esteban Sánchez Ulloa</t>
         </is>
       </c>
       <c r="E69" s="2" t="inlineStr">
@@ -4019,11 +4031,11 @@
       </c>
       <c r="G69" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H69" s="3" t="n">
-        <v>44043.8171875</v>
+        <v>44044.10501157407</v>
       </c>
       <c r="I69" s="2" t="n"/>
       <c r="J69" s="2" t="n"/>
@@ -4039,48 +4051,42 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B70" s="2" t="n">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>198182354</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr">
         <is>
-          <t>Matías Severino</t>
+          <t>Víctor Esteban Sánchez Ulloa</t>
         </is>
       </c>
       <c r="E70" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G70" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H70" s="3" t="n">
-        <v>44043.8171875</v>
-      </c>
-      <c r="I70" s="3" t="n">
-        <v>44043.98478009259</v>
-      </c>
-      <c r="J70" s="3" t="n">
-        <v>44043.75</v>
-      </c>
-      <c r="K70" s="3" t="n">
-        <v>44043.81805555556</v>
-      </c>
+        <v>44044.09211805555</v>
+      </c>
+      <c r="I70" s="2" t="n"/>
+      <c r="J70" s="2" t="n"/>
+      <c r="K70" s="2" t="n"/>
       <c r="L70" s="2" t="n"/>
       <c r="M70" s="2" t="n"/>
       <c r="N70" s="2" t="n"/>
@@ -4092,10 +4098,10 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B71" s="2" t="n">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
@@ -4109,12 +4115,12 @@
       </c>
       <c r="E71" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F71" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G71" s="2" t="inlineStr">
@@ -4123,7 +4129,7 @@
         </is>
       </c>
       <c r="H71" s="3" t="n">
-        <v>44043.80297453704</v>
+        <v>44043.8171875</v>
       </c>
       <c r="I71" s="2" t="n"/>
       <c r="J71" s="2" t="n"/>
@@ -4139,10 +4145,10 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B72" s="2" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
@@ -4156,12 +4162,12 @@
       </c>
       <c r="E72" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G72" s="2" t="inlineStr">
@@ -4170,16 +4176,16 @@
         </is>
       </c>
       <c r="H72" s="3" t="n">
-        <v>44043.80297453704</v>
+        <v>44043.8171875</v>
       </c>
       <c r="I72" s="3" t="n">
-        <v>44043.97052083333</v>
+        <v>44043.98478009259</v>
       </c>
       <c r="J72" s="3" t="n">
-        <v>44053.75</v>
+        <v>44043.75</v>
       </c>
       <c r="K72" s="3" t="n">
-        <v>44043.97069444445</v>
+        <v>44043.81805555556</v>
       </c>
       <c r="L72" s="2" t="n"/>
       <c r="M72" s="2" t="n"/>
@@ -4192,10 +4198,10 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B73" s="2" t="n">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C73" s="2" t="inlineStr">
         <is>
@@ -4223,7 +4229,7 @@
         </is>
       </c>
       <c r="H73" s="3" t="n">
-        <v>44043.52788194444</v>
+        <v>44043.80297453704</v>
       </c>
       <c r="I73" s="2" t="n"/>
       <c r="J73" s="2" t="n"/>
@@ -4239,42 +4245,48 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B74" s="2" t="n">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>12345678</t>
         </is>
       </c>
       <c r="D74" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Matías Severino</t>
         </is>
       </c>
       <c r="E74" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G74" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H74" s="3" t="n">
-        <v>44040.51644675926</v>
-      </c>
-      <c r="I74" s="2" t="n"/>
-      <c r="J74" s="2" t="n"/>
-      <c r="K74" s="2" t="n"/>
+        <v>44043.80297453704</v>
+      </c>
+      <c r="I74" s="3" t="n">
+        <v>44043.97052083333</v>
+      </c>
+      <c r="J74" s="3" t="n">
+        <v>44053.75</v>
+      </c>
+      <c r="K74" s="3" t="n">
+        <v>44043.97069444445</v>
+      </c>
       <c r="L74" s="2" t="n"/>
       <c r="M74" s="2" t="n"/>
       <c r="N74" s="2" t="n"/>
@@ -4286,29 +4298,29 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B75" s="2" t="n">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>12345678</t>
         </is>
       </c>
       <c r="D75" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Matías Severino</t>
         </is>
       </c>
       <c r="E75" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F75" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G75" s="2" t="inlineStr">
@@ -4317,7 +4329,7 @@
         </is>
       </c>
       <c r="H75" s="3" t="n">
-        <v>44040.51644675926</v>
+        <v>44043.52788194444</v>
       </c>
       <c r="I75" s="2" t="n"/>
       <c r="J75" s="2" t="n"/>
@@ -4333,10 +4345,10 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B76" s="2" t="n">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
@@ -4350,12 +4362,12 @@
       </c>
       <c r="E76" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G76" s="2" t="inlineStr">
@@ -4364,7 +4376,7 @@
         </is>
       </c>
       <c r="H76" s="3" t="n">
-        <v>44036.71489583333</v>
+        <v>44040.51644675926</v>
       </c>
       <c r="I76" s="2" t="n"/>
       <c r="J76" s="2" t="n"/>
@@ -4380,10 +4392,10 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B77" s="2" t="n">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
@@ -4397,12 +4409,12 @@
       </c>
       <c r="E77" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F77" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G77" s="2" t="inlineStr">
@@ -4411,7 +4423,7 @@
         </is>
       </c>
       <c r="H77" s="3" t="n">
-        <v>44036.71489583333</v>
+        <v>44040.51644675926</v>
       </c>
       <c r="I77" s="2" t="n"/>
       <c r="J77" s="2" t="n"/>
@@ -4427,10 +4439,10 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B78" s="2" t="n">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
@@ -4444,28 +4456,26 @@
       </c>
       <c r="E78" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G78" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H78" s="3" t="n">
-        <v>44034.65239583333</v>
+        <v>44036.71489583333</v>
       </c>
       <c r="I78" s="2" t="n"/>
       <c r="J78" s="2" t="n"/>
       <c r="K78" s="2" t="n"/>
-      <c r="L78" s="3" t="n">
-        <v>44041</v>
-      </c>
+      <c r="L78" s="2" t="n"/>
       <c r="M78" s="2" t="n"/>
       <c r="N78" s="2" t="n"/>
       <c r="O78" s="2" t="n">
@@ -4476,10 +4486,10 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B79" s="2" t="n">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C79" s="2" t="inlineStr">
         <is>
@@ -4493,31 +4503,25 @@
       </c>
       <c r="E79" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F79" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G79" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H79" s="3" t="n">
-        <v>44031.79657407408</v>
-      </c>
-      <c r="I79" s="3" t="n">
-        <v>44041.55918981481</v>
-      </c>
-      <c r="J79" s="3" t="n">
-        <v>44041.75</v>
-      </c>
-      <c r="K79" s="3" t="n">
-        <v>44049.58769675926</v>
-      </c>
+        <v>44036.71489583333</v>
+      </c>
+      <c r="I79" s="2" t="n"/>
+      <c r="J79" s="2" t="n"/>
+      <c r="K79" s="2" t="n"/>
       <c r="L79" s="2" t="n"/>
       <c r="M79" s="2" t="n"/>
       <c r="N79" s="2" t="n"/>
@@ -4527,6 +4531,108 @@
       <c r="P79" s="2" t="n"/>
       <c r="Q79" s="2" t="n"/>
     </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="B80" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>19889608K</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>Sebastián Ignacio Toro Severino</t>
+        </is>
+      </c>
+      <c r="E80" s="2" t="inlineStr">
+        <is>
+          <t>Celular Samsung Galaxy S4</t>
+        </is>
+      </c>
+      <c r="F80" s="2" t="inlineStr">
+        <is>
+          <t>AAD832</t>
+        </is>
+      </c>
+      <c r="G80" s="2" t="inlineStr">
+        <is>
+          <t>Cancelada</t>
+        </is>
+      </c>
+      <c r="H80" s="3" t="n">
+        <v>44034.65239583333</v>
+      </c>
+      <c r="I80" s="2" t="n"/>
+      <c r="J80" s="2" t="n"/>
+      <c r="K80" s="2" t="n"/>
+      <c r="L80" s="3" t="n">
+        <v>44041</v>
+      </c>
+      <c r="M80" s="2" t="n"/>
+      <c r="N80" s="2" t="n"/>
+      <c r="O80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P80" s="2" t="n"/>
+      <c r="Q80" s="2" t="n"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="B81" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="C81" s="2" t="inlineStr">
+        <is>
+          <t>19889608K</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>Sebastián Ignacio Toro Severino</t>
+        </is>
+      </c>
+      <c r="E81" s="2" t="inlineStr">
+        <is>
+          <t>Drone Parrot Bebop 2</t>
+        </is>
+      </c>
+      <c r="F81" s="2" t="inlineStr">
+        <is>
+          <t>ABC432</t>
+        </is>
+      </c>
+      <c r="G81" s="2" t="inlineStr">
+        <is>
+          <t>Finalizada</t>
+        </is>
+      </c>
+      <c r="H81" s="3" t="n">
+        <v>44031.79657407408</v>
+      </c>
+      <c r="I81" s="3" t="n">
+        <v>44041.55918981481</v>
+      </c>
+      <c r="J81" s="3" t="n">
+        <v>44041.75</v>
+      </c>
+      <c r="K81" s="3" t="n">
+        <v>44049.58769675926</v>
+      </c>
+      <c r="L81" s="2" t="n"/>
+      <c r="M81" s="2" t="n"/>
+      <c r="N81" s="2" t="n"/>
+      <c r="O81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" s="2" t="n"/>
+      <c r="Q81" s="2" t="n"/>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
apscheduler desplazado fuera de la app
</commit_message>
<xml_diff>
--- a/flask/app/static/files/exportaciones/historial_solicitudes.xlsx
+++ b/flask/app/static/files/exportaciones/historial_solicitudes.xlsx
@@ -564,19 +564,19 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>798</v>
+        <v>826</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -591,30 +591,37 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H2" s="3" t="n">
-        <v>44110.41626157407</v>
+        <v>44110.98806712963</v>
       </c>
       <c r="I2" s="2" t="n"/>
       <c r="J2" s="2" t="n"/>
       <c r="K2" s="2" t="n"/>
       <c r="L2" s="2" t="n"/>
-      <c r="M2" s="2" t="n"/>
+      <c r="M2" s="3" t="n">
+        <v>44113.00635416667</v>
+      </c>
       <c r="N2" s="2" t="n"/>
       <c r="O2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P2" s="2" t="n"/>
+      <c r="P2" s="2" t="inlineStr">
+        <is>
+          <t>Pasó mucho tiempo,
+Saludos</t>
+        </is>
+      </c>
       <c r="Q2" s="2" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>793</v>
+        <v>798</v>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
@@ -628,12 +635,12 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
@@ -642,7 +649,7 @@
         </is>
       </c>
       <c r="H3" s="3" t="n">
-        <v>44110.0515162037</v>
+        <v>44110.41626157407</v>
       </c>
       <c r="I3" s="2" t="n"/>
       <c r="J3" s="2" t="n"/>
@@ -661,7 +668,7 @@
         <v>254</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
@@ -705,10 +712,10 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>790</v>
+        <v>796</v>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
@@ -722,12 +729,12 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
@@ -736,7 +743,7 @@
         </is>
       </c>
       <c r="H5" s="3" t="n">
-        <v>44109.79221064815</v>
+        <v>44110.0515162037</v>
       </c>
       <c r="I5" s="2" t="n"/>
       <c r="J5" s="2" t="n"/>
@@ -752,10 +759,10 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>785</v>
+        <v>790</v>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
@@ -769,12 +776,12 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G6" s="2" t="inlineStr">
@@ -783,7 +790,7 @@
         </is>
       </c>
       <c r="H6" s="3" t="n">
-        <v>44109.47980324074</v>
+        <v>44109.79221064815</v>
       </c>
       <c r="I6" s="2" t="n"/>
       <c r="J6" s="2" t="n"/>
@@ -799,29 +806,29 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
@@ -830,7 +837,7 @@
         </is>
       </c>
       <c r="H7" s="3" t="n">
-        <v>44109.12380787037</v>
+        <v>44109.47980324074</v>
       </c>
       <c r="I7" s="2" t="n"/>
       <c r="J7" s="2" t="n"/>
@@ -846,29 +853,29 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
@@ -877,7 +884,7 @@
         </is>
       </c>
       <c r="H8" s="3" t="n">
-        <v>44109.04577546296</v>
+        <v>44109.12380787037</v>
       </c>
       <c r="I8" s="2" t="n"/>
       <c r="J8" s="2" t="n"/>
@@ -893,29 +900,29 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>774</v>
+        <v>780</v>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>Modulo Wifi Heltecs LoRa 32</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>ADM123</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G9" s="2" t="inlineStr">
@@ -924,53 +931,45 @@
         </is>
       </c>
       <c r="H9" s="3" t="n">
-        <v>44108.92686342593</v>
+        <v>44109.04577546296</v>
       </c>
       <c r="I9" s="2" t="n"/>
       <c r="J9" s="2" t="n"/>
       <c r="K9" s="2" t="n"/>
-      <c r="L9" s="3" t="n">
-        <v>44109.77083333334</v>
-      </c>
+      <c r="L9" s="2" t="n"/>
       <c r="M9" s="2" t="n"/>
-      <c r="N9" s="3" t="n">
-        <v>44110.02006944444</v>
-      </c>
+      <c r="N9" s="2" t="n"/>
       <c r="O9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P9" s="2" t="inlineStr">
-        <is>
-          <t>Cancelada por sanción, lo siento :o</t>
-        </is>
-      </c>
+      <c r="P9" s="2" t="n"/>
       <c r="Q9" s="2" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>764</v>
+        <v>774</v>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>196378081</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>Nicolás Felipe Opazo Gana</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Modulo Wifi Heltecs LoRa 32</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>ADM123</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr">
@@ -979,18 +978,26 @@
         </is>
       </c>
       <c r="H10" s="3" t="n">
-        <v>44108.05787037037</v>
+        <v>44108.92686342593</v>
       </c>
       <c r="I10" s="2" t="n"/>
       <c r="J10" s="2" t="n"/>
       <c r="K10" s="2" t="n"/>
-      <c r="L10" s="2" t="n"/>
+      <c r="L10" s="3" t="n">
+        <v>44109.77083333334</v>
+      </c>
       <c r="M10" s="2" t="n"/>
-      <c r="N10" s="2" t="n"/>
+      <c r="N10" s="3" t="n">
+        <v>44110.02006944444</v>
+      </c>
       <c r="O10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P10" s="2" t="n"/>
+      <c r="P10" s="2" t="inlineStr">
+        <is>
+          <t>Cancelada por sanción, lo siento :o</t>
+        </is>
+      </c>
       <c r="Q10" s="2" t="n"/>
     </row>
     <row r="11">
@@ -998,7 +1005,7 @@
         <v>244</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
@@ -1042,29 +1049,29 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>734</v>
+        <v>763</v>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>196378081</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Nicolás Felipe Opazo Gana</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Modulo Wifi Heltecs LoRa 32</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>ADM123</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
@@ -1073,7 +1080,7 @@
         </is>
       </c>
       <c r="H12" s="3" t="n">
-        <v>44108.03136574074</v>
+        <v>44108.05787037037</v>
       </c>
       <c r="I12" s="2" t="n"/>
       <c r="J12" s="2" t="n"/>
@@ -1092,7 +1099,7 @@
         <v>243</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
@@ -1106,17 +1113,17 @@
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Modulo Wifi Heltecs LoRa 32</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>ADM123</t>
         </is>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H13" s="3" t="n">
@@ -1126,27 +1133,20 @@
       <c r="J13" s="2" t="n"/>
       <c r="K13" s="2" t="n"/>
       <c r="L13" s="2" t="n"/>
-      <c r="M13" s="3" t="n">
-        <v>44108.0318287037</v>
-      </c>
+      <c r="M13" s="2" t="n"/>
       <c r="N13" s="2" t="n"/>
       <c r="O13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P13" s="2" t="inlineStr">
-        <is>
-          <t>Me queda una última placa y la tenía reservada a otra persona.
-Prueba mañana!</t>
-        </is>
-      </c>
+      <c r="P13" s="2" t="n"/>
       <c r="Q13" s="2" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>727</v>
+        <v>735</v>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
@@ -1160,32 +1160,39 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H14" s="3" t="n">
-        <v>44108.02136574074</v>
+        <v>44108.03136574074</v>
       </c>
       <c r="I14" s="2" t="n"/>
       <c r="J14" s="2" t="n"/>
       <c r="K14" s="2" t="n"/>
       <c r="L14" s="2" t="n"/>
-      <c r="M14" s="2" t="n"/>
+      <c r="M14" s="3" t="n">
+        <v>44108.0318287037</v>
+      </c>
       <c r="N14" s="2" t="n"/>
       <c r="O14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P14" s="2" t="n"/>
+      <c r="P14" s="2" t="inlineStr">
+        <is>
+          <t>Me queda una última placa y la tenía reservada a otra persona.
+Prueba mañana!</t>
+        </is>
+      </c>
       <c r="Q14" s="2" t="n"/>
     </row>
     <row r="15">
@@ -1193,7 +1200,7 @@
         <v>242</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
@@ -1207,31 +1214,25 @@
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H15" s="3" t="n">
         <v>44108.02136574074</v>
       </c>
-      <c r="I15" s="3" t="n">
-        <v>44108.02583333333</v>
-      </c>
-      <c r="J15" s="3" t="n">
-        <v>44109.77083333334</v>
-      </c>
-      <c r="K15" s="3" t="n">
-        <v>44109.81986111111</v>
-      </c>
+      <c r="I15" s="2" t="n"/>
+      <c r="J15" s="2" t="n"/>
+      <c r="K15" s="2" t="n"/>
       <c r="L15" s="2" t="n"/>
       <c r="M15" s="2" t="n"/>
       <c r="N15" s="2" t="n"/>
@@ -1246,7 +1247,7 @@
         <v>242</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
@@ -1260,25 +1261,31 @@
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H16" s="3" t="n">
         <v>44108.02136574074</v>
       </c>
-      <c r="I16" s="2" t="n"/>
-      <c r="J16" s="2" t="n"/>
-      <c r="K16" s="2" t="n"/>
+      <c r="I16" s="3" t="n">
+        <v>44108.02583333333</v>
+      </c>
+      <c r="J16" s="3" t="n">
+        <v>44109.77083333334</v>
+      </c>
+      <c r="K16" s="3" t="n">
+        <v>44109.81986111111</v>
+      </c>
       <c r="L16" s="2" t="n"/>
       <c r="M16" s="2" t="n"/>
       <c r="N16" s="2" t="n"/>
@@ -1290,10 +1297,10 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>718</v>
+        <v>732</v>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
@@ -1307,31 +1314,25 @@
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H17" s="3" t="n">
-        <v>44107.69290509259</v>
-      </c>
-      <c r="I17" s="3" t="n">
-        <v>44107.69290509259</v>
-      </c>
-      <c r="J17" s="3" t="n">
-        <v>44119.77083333334</v>
-      </c>
-      <c r="K17" s="3" t="n">
-        <v>44107.70171296296</v>
-      </c>
+        <v>44108.02136574074</v>
+      </c>
+      <c r="I17" s="2" t="n"/>
+      <c r="J17" s="2" t="n"/>
+      <c r="K17" s="2" t="n"/>
       <c r="L17" s="2" t="n"/>
       <c r="M17" s="2" t="n"/>
       <c r="N17" s="2" t="n"/>
@@ -1343,10 +1344,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
@@ -1360,48 +1361,46 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Modulo Wifi Heltecs LoRa 32</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>ADM123</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H18" s="3" t="n">
-        <v>44107.6053125</v>
-      </c>
-      <c r="I18" s="2" t="n"/>
-      <c r="J18" s="2" t="n"/>
-      <c r="K18" s="2" t="n"/>
-      <c r="L18" s="3" t="n">
-        <v>44110.77083333334</v>
-      </c>
+        <v>44107.69290509259</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <v>44107.69290509259</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <v>44119.77083333334</v>
+      </c>
+      <c r="K18" s="3" t="n">
+        <v>44107.70171296296</v>
+      </c>
+      <c r="L18" s="2" t="n"/>
       <c r="M18" s="2" t="n"/>
-      <c r="N18" s="3" t="n">
-        <v>44108.02855324074</v>
-      </c>
+      <c r="N18" s="2" t="n"/>
       <c r="O18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P18" s="2" t="inlineStr">
-        <is>
-          <t>Cancelado por motivos internos, intenta para la próxima!</t>
-        </is>
-      </c>
+      <c r="P18" s="2" t="n"/>
       <c r="Q18" s="2" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>697</v>
+        <v>716</v>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
@@ -1415,46 +1414,48 @@
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Modulo Wifi Heltecs LoRa 32</t>
         </is>
       </c>
       <c r="F19" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>ADM123</t>
         </is>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H19" s="3" t="n">
-        <v>44107.56030092593</v>
+        <v>44107.6053125</v>
       </c>
       <c r="I19" s="2" t="n"/>
       <c r="J19" s="2" t="n"/>
       <c r="K19" s="2" t="n"/>
-      <c r="L19" s="2" t="n"/>
-      <c r="M19" s="3" t="n">
-        <v>44107.58023148148</v>
-      </c>
-      <c r="N19" s="2" t="n"/>
+      <c r="L19" s="3" t="n">
+        <v>44110.77083333334</v>
+      </c>
+      <c r="M19" s="2" t="n"/>
+      <c r="N19" s="3" t="n">
+        <v>44108.02855324074</v>
+      </c>
       <c r="O19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="P19" s="2" t="inlineStr">
         <is>
-          <t>Sin stock</t>
+          <t>Cancelado por motivos internos, intenta para la próxima!</t>
         </is>
       </c>
       <c r="Q19" s="2" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>627</v>
+        <v>697</v>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
@@ -1468,49 +1469,46 @@
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H20" s="3" t="n">
-        <v>44105.72270833333</v>
+        <v>44107.56030092593</v>
       </c>
       <c r="I20" s="2" t="n"/>
       <c r="J20" s="2" t="n"/>
       <c r="K20" s="2" t="n"/>
-      <c r="L20" s="3" t="n">
-        <v>44111.77083333334</v>
-      </c>
-      <c r="M20" s="2" t="n"/>
-      <c r="N20" s="3" t="n">
-        <v>44108.0268287037</v>
-      </c>
+      <c r="L20" s="2" t="n"/>
+      <c r="M20" s="3" t="n">
+        <v>44107.58023148148</v>
+      </c>
+      <c r="N20" s="2" t="n"/>
       <c r="O20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="P20" s="2" t="inlineStr">
         <is>
-          <t>Motivos internos
-Lo siento :c</t>
+          <t>Sin stock</t>
         </is>
       </c>
       <c r="Q20" s="2" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
@@ -1538,106 +1536,109 @@
         </is>
       </c>
       <c r="H21" s="3" t="n">
-        <v>44105.7222800926</v>
+        <v>44105.72270833333</v>
       </c>
       <c r="I21" s="2" t="n"/>
       <c r="J21" s="2" t="n"/>
       <c r="K21" s="2" t="n"/>
       <c r="L21" s="3" t="n">
-        <v>44110.77083333334</v>
+        <v>44111.77083333334</v>
       </c>
       <c r="M21" s="2" t="n"/>
       <c r="N21" s="3" t="n">
-        <v>44105.72297453704</v>
+        <v>44108.0268287037</v>
       </c>
       <c r="O21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="P21" s="2" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>Motivos internos
+Lo siento :c</t>
         </is>
       </c>
       <c r="Q21" s="2" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H22" s="3" t="n">
-        <v>44105.06001157407</v>
-      </c>
-      <c r="I22" s="3" t="n">
-        <v>44105.06001157407</v>
-      </c>
-      <c r="J22" s="3" t="n">
+        <v>44105.7222800926</v>
+      </c>
+      <c r="I22" s="2" t="n"/>
+      <c r="J22" s="2" t="n"/>
+      <c r="K22" s="2" t="n"/>
+      <c r="L22" s="3" t="n">
         <v>44110.77083333334</v>
       </c>
-      <c r="K22" s="3" t="n">
-        <v>44110.99744212963</v>
-      </c>
-      <c r="L22" s="2" t="n"/>
       <c r="M22" s="2" t="n"/>
-      <c r="N22" s="2" t="n"/>
+      <c r="N22" s="3" t="n">
+        <v>44105.72297453704</v>
+      </c>
       <c r="O22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P22" s="2" t="n"/>
+      <c r="P22" s="2" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="Q22" s="2" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>611</v>
+        <v>622</v>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F23" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G23" s="2" t="inlineStr">
@@ -1646,16 +1647,16 @@
         </is>
       </c>
       <c r="H23" s="3" t="n">
-        <v>44104.53206018519</v>
+        <v>44105.06001157407</v>
       </c>
       <c r="I23" s="3" t="n">
-        <v>44104.55636574074</v>
+        <v>44105.06001157407</v>
       </c>
       <c r="J23" s="3" t="n">
-        <v>44104.77083333334</v>
+        <v>44110.77083333334</v>
       </c>
       <c r="K23" s="3" t="n">
-        <v>44104.78267361111</v>
+        <v>44110.99744212963</v>
       </c>
       <c r="L23" s="2" t="n"/>
       <c r="M23" s="2" t="n"/>
@@ -1668,10 +1669,10 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
@@ -1685,12 +1686,12 @@
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G24" s="2" t="inlineStr">
@@ -1699,16 +1700,16 @@
         </is>
       </c>
       <c r="H24" s="3" t="n">
-        <v>44104.07725694445</v>
+        <v>44104.53206018519</v>
       </c>
       <c r="I24" s="3" t="n">
-        <v>44104.49207175926</v>
+        <v>44104.55636574074</v>
       </c>
       <c r="J24" s="3" t="n">
-        <v>44106.77083333334</v>
+        <v>44104.77083333334</v>
       </c>
       <c r="K24" s="3" t="n">
-        <v>44105.03828703704</v>
+        <v>44104.78267361111</v>
       </c>
       <c r="L24" s="2" t="n"/>
       <c r="M24" s="2" t="n"/>
@@ -1721,19 +1722,19 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr">
@@ -1752,16 +1753,16 @@
         </is>
       </c>
       <c r="H25" s="3" t="n">
-        <v>44104.06814814815</v>
+        <v>44104.07725694445</v>
       </c>
       <c r="I25" s="3" t="n">
-        <v>44104.07643518518</v>
+        <v>44104.49207175926</v>
       </c>
       <c r="J25" s="3" t="n">
-        <v>44116.77083333334</v>
+        <v>44106.77083333334</v>
       </c>
       <c r="K25" s="3" t="n">
-        <v>44108.02783564815</v>
+        <v>44105.03828703704</v>
       </c>
       <c r="L25" s="2" t="n"/>
       <c r="M25" s="2" t="n"/>
@@ -1774,10 +1775,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
@@ -1791,12 +1792,12 @@
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G26" s="2" t="inlineStr">
@@ -1805,16 +1806,16 @@
         </is>
       </c>
       <c r="H26" s="3" t="n">
-        <v>44103.99357638889</v>
+        <v>44104.06814814815</v>
       </c>
       <c r="I26" s="3" t="n">
-        <v>44103.99490740741</v>
+        <v>44104.07643518518</v>
       </c>
       <c r="J26" s="3" t="n">
-        <v>44103.77083333334</v>
+        <v>44116.77083333334</v>
       </c>
       <c r="K26" s="3" t="n">
-        <v>44104.003125</v>
+        <v>44108.02783564815</v>
       </c>
       <c r="L26" s="2" t="n"/>
       <c r="M26" s="2" t="n"/>
@@ -1827,57 +1828,55 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F27" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H27" s="3" t="n">
-        <v>44103.99023148148</v>
-      </c>
-      <c r="I27" s="2" t="n"/>
-      <c r="J27" s="2" t="n"/>
-      <c r="K27" s="2" t="n"/>
-      <c r="L27" s="3" t="n">
+        <v>44103.99357638889</v>
+      </c>
+      <c r="I27" s="3" t="n">
+        <v>44103.99490740741</v>
+      </c>
+      <c r="J27" s="3" t="n">
         <v>44103.77083333334</v>
       </c>
+      <c r="K27" s="3" t="n">
+        <v>44104.003125</v>
+      </c>
+      <c r="L27" s="2" t="n"/>
       <c r="M27" s="2" t="n"/>
-      <c r="N27" s="3" t="n">
-        <v>44104.06228009259</v>
-      </c>
+      <c r="N27" s="2" t="n"/>
       <c r="O27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P27" s="2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
+      <c r="P27" s="2" t="n"/>
       <c r="Q27" s="2" t="n"/>
     </row>
     <row r="28">
@@ -1885,7 +1884,7 @@
         <v>201</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
@@ -1899,65 +1898,67 @@
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H28" s="3" t="n">
         <v>44103.99023148148</v>
       </c>
-      <c r="I28" s="3" t="n">
-        <v>44103.9909837963</v>
-      </c>
-      <c r="J28" s="3" t="n">
+      <c r="I28" s="2" t="n"/>
+      <c r="J28" s="2" t="n"/>
+      <c r="K28" s="2" t="n"/>
+      <c r="L28" s="3" t="n">
         <v>44103.77083333334</v>
       </c>
-      <c r="K28" s="3" t="n">
-        <v>44104.55571759259</v>
-      </c>
-      <c r="L28" s="2" t="n"/>
       <c r="M28" s="2" t="n"/>
-      <c r="N28" s="2" t="n"/>
+      <c r="N28" s="3" t="n">
+        <v>44104.06228009259</v>
+      </c>
       <c r="O28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="P28" s="2" t="n"/>
+      <c r="P28" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
       <c r="Q28" s="2" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>583</v>
+        <v>599</v>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G29" s="2" t="inlineStr">
@@ -1966,16 +1967,16 @@
         </is>
       </c>
       <c r="H29" s="3" t="n">
-        <v>44100.91527777778</v>
+        <v>44103.99023148148</v>
       </c>
       <c r="I29" s="3" t="n">
-        <v>44103.82704861111</v>
+        <v>44103.9909837963</v>
       </c>
       <c r="J29" s="3" t="n">
-        <v>44106.77083333334</v>
+        <v>44103.77083333334</v>
       </c>
       <c r="K29" s="3" t="n">
-        <v>44103.84380787037</v>
+        <v>44104.55571759259</v>
       </c>
       <c r="L29" s="2" t="n"/>
       <c r="M29" s="2" t="n"/>
@@ -1988,10 +1989,10 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
@@ -2005,12 +2006,12 @@
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G30" s="2" t="inlineStr">
@@ -2019,16 +2020,16 @@
         </is>
       </c>
       <c r="H30" s="3" t="n">
-        <v>44100.04094907407</v>
+        <v>44100.91527777778</v>
       </c>
       <c r="I30" s="3" t="n">
-        <v>44100.04094907407</v>
+        <v>44103.82704861111</v>
       </c>
       <c r="J30" s="3" t="n">
-        <v>44102.77083333334</v>
+        <v>44106.77083333334</v>
       </c>
       <c r="K30" s="3" t="n">
-        <v>44100.90773148148</v>
+        <v>44103.84380787037</v>
       </c>
       <c r="L30" s="2" t="n"/>
       <c r="M30" s="2" t="n"/>
@@ -2044,7 +2045,7 @@
         <v>193</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
@@ -2058,12 +2059,12 @@
       </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G31" s="2" t="inlineStr">
@@ -2081,7 +2082,7 @@
         <v>44102.77083333334</v>
       </c>
       <c r="K31" s="3" t="n">
-        <v>44102.02782407407</v>
+        <v>44100.90773148148</v>
       </c>
       <c r="L31" s="2" t="n"/>
       <c r="M31" s="2" t="n"/>
@@ -2094,19 +2095,19 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E32" s="2" t="inlineStr">
@@ -2125,16 +2126,16 @@
         </is>
       </c>
       <c r="H32" s="3" t="n">
-        <v>44100.03137731482</v>
+        <v>44100.04094907407</v>
       </c>
       <c r="I32" s="3" t="n">
-        <v>44100.03137731482</v>
+        <v>44100.04094907407</v>
       </c>
       <c r="J32" s="3" t="n">
-        <v>44104.77083333334</v>
+        <v>44102.77083333334</v>
       </c>
       <c r="K32" s="3" t="n">
-        <v>44103.90252314815</v>
+        <v>44102.02782407407</v>
       </c>
       <c r="L32" s="2" t="n"/>
       <c r="M32" s="2" t="n"/>
@@ -2147,10 +2148,10 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
@@ -2164,12 +2165,12 @@
       </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F33" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G33" s="2" t="inlineStr">
@@ -2178,16 +2179,16 @@
         </is>
       </c>
       <c r="H33" s="3" t="n">
-        <v>44099.99474537037</v>
+        <v>44100.03137731482</v>
       </c>
       <c r="I33" s="3" t="n">
-        <v>44099.99474537037</v>
+        <v>44100.03137731482</v>
       </c>
       <c r="J33" s="3" t="n">
-        <v>44102.77083333334</v>
+        <v>44104.77083333334</v>
       </c>
       <c r="K33" s="3" t="n">
-        <v>44102.02828703704</v>
+        <v>44103.90252314815</v>
       </c>
       <c r="L33" s="2" t="n"/>
       <c r="M33" s="2" t="n"/>
@@ -2200,10 +2201,10 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>554</v>
+        <v>572</v>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
@@ -2217,12 +2218,12 @@
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G34" s="2" t="inlineStr">
@@ -2231,32 +2232,32 @@
         </is>
       </c>
       <c r="H34" s="3" t="n">
-        <v>44099.56803240741</v>
+        <v>44099.99474537037</v>
       </c>
       <c r="I34" s="3" t="n">
-        <v>44099.6490162037</v>
+        <v>44099.99474537037</v>
       </c>
       <c r="J34" s="3" t="n">
-        <v>44109.77083333334</v>
+        <v>44102.77083333334</v>
       </c>
       <c r="K34" s="3" t="n">
-        <v>44103.90502314815</v>
+        <v>44102.02828703704</v>
       </c>
       <c r="L34" s="2" t="n"/>
       <c r="M34" s="2" t="n"/>
       <c r="N34" s="2" t="n"/>
       <c r="O34" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34" s="2" t="n"/>
       <c r="Q34" s="2" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>508</v>
+        <v>554</v>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
@@ -2280,29 +2281,28 @@
       </c>
       <c r="G35" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H35" s="3" t="n">
-        <v>44094.73216435185</v>
-      </c>
-      <c r="I35" s="2" t="n"/>
-      <c r="J35" s="2" t="n"/>
-      <c r="K35" s="2" t="n"/>
+        <v>44099.56803240741</v>
+      </c>
+      <c r="I35" s="3" t="n">
+        <v>44099.6490162037</v>
+      </c>
+      <c r="J35" s="3" t="n">
+        <v>44109.77083333334</v>
+      </c>
+      <c r="K35" s="3" t="n">
+        <v>44103.90502314815</v>
+      </c>
       <c r="L35" s="2" t="n"/>
-      <c r="M35" s="3" t="n">
-        <v>44094.75707175926</v>
-      </c>
+      <c r="M35" s="2" t="n"/>
       <c r="N35" s="2" t="n"/>
       <c r="O35" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P35" s="2" t="inlineStr">
-        <is>
-          <t>Prueba de rechazo de solicitud
-LabEIT.-</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="P35" s="2" t="n"/>
       <c r="Q35" s="2" t="n"/>
     </row>
     <row r="36">
@@ -2310,7 +2310,7 @@
         <v>154</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
@@ -2324,17 +2324,17 @@
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G36" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H36" s="3" t="n">
@@ -2343,139 +2343,140 @@
       <c r="I36" s="2" t="n"/>
       <c r="J36" s="2" t="n"/>
       <c r="K36" s="2" t="n"/>
-      <c r="L36" s="3" t="n">
+      <c r="L36" s="2" t="n"/>
+      <c r="M36" s="3" t="n">
+        <v>44094.75707175926</v>
+      </c>
+      <c r="N36" s="2" t="n"/>
+      <c r="O36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" s="2" t="inlineStr">
+        <is>
+          <t>Prueba de rechazo de solicitud
+LabEIT.-</t>
+        </is>
+      </c>
+      <c r="Q36" s="2" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>154</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>510</v>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>19889608K</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>Sebastián Ignacio Toro Severino</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>Router TP-LINK TL-WN722N</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>AAA351</t>
+        </is>
+      </c>
+      <c r="G37" s="2" t="inlineStr">
+        <is>
+          <t>Cancelada</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>44094.73216435185</v>
+      </c>
+      <c r="I37" s="2" t="n"/>
+      <c r="J37" s="2" t="n"/>
+      <c r="K37" s="2" t="n"/>
+      <c r="L37" s="3" t="n">
         <v>44096.77083333334</v>
       </c>
-      <c r="M36" s="2" t="n"/>
-      <c r="N36" s="3" t="n">
+      <c r="M37" s="2" t="n"/>
+      <c r="N37" s="3" t="n">
         <v>44094.73256944444</v>
       </c>
-      <c r="O36" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P36" s="2" t="inlineStr">
+      <c r="O37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2" t="inlineStr">
         <is>
           <t>Cancelación de prueba
 LabEIT
 2020</t>
         </is>
       </c>
-      <c r="Q36" s="2" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
+      <c r="Q37" s="2" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
         <v>154</v>
       </c>
-      <c r="B37" s="2" t="n">
+      <c r="B38" s="2" t="n">
         <v>511</v>
       </c>
-      <c r="C37" s="2" t="inlineStr">
+      <c r="C38" s="2" t="inlineStr">
         <is>
           <t>19889608K</t>
         </is>
       </c>
-      <c r="D37" s="2" t="inlineStr">
+      <c r="D38" s="2" t="inlineStr">
         <is>
           <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
-      <c r="E37" s="2" t="inlineStr">
+      <c r="E38" s="2" t="inlineStr">
         <is>
           <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
-      <c r="F37" s="2" t="inlineStr">
+      <c r="F38" s="2" t="inlineStr">
         <is>
           <t>AAA351</t>
         </is>
       </c>
-      <c r="G37" s="2" t="inlineStr">
+      <c r="G38" s="2" t="inlineStr">
         <is>
           <t>Rechazada</t>
         </is>
       </c>
-      <c r="H37" s="3" t="n">
+      <c r="H38" s="3" t="n">
         <v>44094.73216435185</v>
       </c>
-      <c r="I37" s="2" t="n"/>
-      <c r="J37" s="2" t="n"/>
-      <c r="K37" s="2" t="n"/>
-      <c r="L37" s="2" t="n"/>
-      <c r="M37" s="3" t="n">
+      <c r="I38" s="2" t="n"/>
+      <c r="J38" s="2" t="n"/>
+      <c r="K38" s="2" t="n"/>
+      <c r="L38" s="2" t="n"/>
+      <c r="M38" s="3" t="n">
         <v>44094.73327546296</v>
       </c>
-      <c r="N37" s="2" t="n"/>
-      <c r="O37" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" s="2" t="inlineStr">
+      <c r="N38" s="2" t="n"/>
+      <c r="O38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" s="2" t="inlineStr">
         <is>
           <t>Prueba de rechazo
 LabEIT
 2020</t>
         </is>
       </c>
-      <c r="Q37" s="2" t="n"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="n">
-        <v>87</v>
-      </c>
-      <c r="B38" s="2" t="n">
-        <v>294</v>
-      </c>
-      <c r="C38" s="2" t="inlineStr">
-        <is>
-          <t>19988806K</t>
-        </is>
-      </c>
-      <c r="D38" s="2" t="inlineStr">
-        <is>
-          <t>Sebastián Toro</t>
-        </is>
-      </c>
-      <c r="E38" s="2" t="inlineStr">
-        <is>
-          <t>Notebook  Asus 636-512</t>
-        </is>
-      </c>
-      <c r="F38" s="2" t="inlineStr">
-        <is>
-          <t>ZZZZZ6</t>
-        </is>
-      </c>
-      <c r="G38" s="2" t="inlineStr">
-        <is>
-          <t>Finalizada</t>
-        </is>
-      </c>
-      <c r="H38" s="3" t="n">
-        <v>44068.93978009259</v>
-      </c>
-      <c r="I38" s="3" t="n">
-        <v>44068.98197916667</v>
-      </c>
-      <c r="J38" s="3" t="n">
-        <v>44068.77083333334</v>
-      </c>
-      <c r="K38" s="3" t="n">
-        <v>44068.98927083334</v>
-      </c>
-      <c r="L38" s="2" t="n"/>
-      <c r="M38" s="2" t="n"/>
-      <c r="N38" s="2" t="n"/>
-      <c r="O38" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P38" s="2" t="n"/>
       <c r="Q38" s="2" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
@@ -2489,12 +2490,12 @@
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F39" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G39" s="2" t="inlineStr">
@@ -2503,16 +2504,16 @@
         </is>
       </c>
       <c r="H39" s="3" t="n">
-        <v>44068.903125</v>
+        <v>44068.93978009259</v>
       </c>
       <c r="I39" s="3" t="n">
-        <v>44068.98976851852</v>
+        <v>44068.98197916667</v>
       </c>
       <c r="J39" s="3" t="n">
         <v>44068.77083333334</v>
       </c>
       <c r="K39" s="3" t="n">
-        <v>44068.99473379629</v>
+        <v>44068.98927083334</v>
       </c>
       <c r="L39" s="2" t="n"/>
       <c r="M39" s="2" t="n"/>
@@ -2525,10 +2526,10 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
@@ -2542,12 +2543,12 @@
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G40" s="2" t="inlineStr">
@@ -2556,16 +2557,16 @@
         </is>
       </c>
       <c r="H40" s="3" t="n">
-        <v>44068.63998842592</v>
+        <v>44068.903125</v>
       </c>
       <c r="I40" s="3" t="n">
-        <v>44068.94631944445</v>
+        <v>44068.98976851852</v>
       </c>
       <c r="J40" s="3" t="n">
-        <v>44081.77083333334</v>
+        <v>44068.77083333334</v>
       </c>
       <c r="K40" s="3" t="n">
-        <v>44072.94930555556</v>
+        <v>44068.99473379629</v>
       </c>
       <c r="L40" s="2" t="n"/>
       <c r="M40" s="2" t="n"/>
@@ -2578,10 +2579,10 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
@@ -2595,32 +2596,34 @@
       </c>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G41" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H41" s="3" t="n">
-        <v>44067.97563657408</v>
-      </c>
-      <c r="I41" s="2" t="n"/>
-      <c r="J41" s="2" t="n"/>
-      <c r="K41" s="2" t="n"/>
-      <c r="L41" s="3" t="n">
-        <v>44069.77083333334</v>
-      </c>
+        <v>44068.63998842592</v>
+      </c>
+      <c r="I41" s="3" t="n">
+        <v>44068.94631944445</v>
+      </c>
+      <c r="J41" s="3" t="n">
+        <v>44081.77083333334</v>
+      </c>
+      <c r="K41" s="3" t="n">
+        <v>44072.94930555556</v>
+      </c>
+      <c r="L41" s="2" t="n"/>
       <c r="M41" s="2" t="n"/>
-      <c r="N41" s="3" t="n">
-        <v>44068.02151620371</v>
-      </c>
+      <c r="N41" s="2" t="n"/>
       <c r="O41" s="2" t="n">
         <v>0</v>
       </c>
@@ -2629,10 +2632,10 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
@@ -2646,30 +2649,32 @@
       </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G42" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H42" s="3" t="n">
-        <v>44067.97258101852</v>
+        <v>44067.97563657408</v>
       </c>
       <c r="I42" s="2" t="n"/>
       <c r="J42" s="2" t="n"/>
       <c r="K42" s="2" t="n"/>
-      <c r="L42" s="2" t="n"/>
-      <c r="M42" s="3" t="n">
-        <v>44068.01609953704</v>
-      </c>
-      <c r="N42" s="2" t="n"/>
+      <c r="L42" s="3" t="n">
+        <v>44069.77083333334</v>
+      </c>
+      <c r="M42" s="2" t="n"/>
+      <c r="N42" s="3" t="n">
+        <v>44068.02151620371</v>
+      </c>
       <c r="O42" s="2" t="n">
         <v>0</v>
       </c>
@@ -2681,7 +2686,7 @@
         <v>83</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
@@ -2695,12 +2700,12 @@
       </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G43" s="2" t="inlineStr">
@@ -2716,7 +2721,7 @@
       <c r="K43" s="2" t="n"/>
       <c r="L43" s="2" t="n"/>
       <c r="M43" s="3" t="n">
-        <v>44068.01634259259</v>
+        <v>44068.01609953704</v>
       </c>
       <c r="N43" s="2" t="n"/>
       <c r="O43" s="2" t="n">
@@ -2727,10 +2732,10 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
@@ -2744,36 +2749,32 @@
       </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H44" s="3" t="n">
-        <v>44067.96421296296</v>
-      </c>
-      <c r="I44" s="3" t="n">
-        <v>44068.00895833333</v>
-      </c>
-      <c r="J44" s="3" t="n">
-        <v>44075.77083333334</v>
-      </c>
-      <c r="K44" s="3" t="n">
-        <v>44068.93479166667</v>
-      </c>
+        <v>44067.97258101852</v>
+      </c>
+      <c r="I44" s="2" t="n"/>
+      <c r="J44" s="2" t="n"/>
+      <c r="K44" s="2" t="n"/>
       <c r="L44" s="2" t="n"/>
-      <c r="M44" s="2" t="n"/>
+      <c r="M44" s="3" t="n">
+        <v>44068.01634259259</v>
+      </c>
       <c r="N44" s="2" t="n"/>
       <c r="O44" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P44" s="2" t="n"/>
       <c r="Q44" s="2" t="n"/>
@@ -2783,7 +2784,7 @@
         <v>82</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
@@ -2797,12 +2798,12 @@
       </c>
       <c r="E45" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G45" s="2" t="inlineStr">
@@ -2814,29 +2815,29 @@
         <v>44067.96421296296</v>
       </c>
       <c r="I45" s="3" t="n">
-        <v>44068.99569444444</v>
+        <v>44068.00895833333</v>
       </c>
       <c r="J45" s="3" t="n">
-        <v>44068.77083333334</v>
+        <v>44075.77083333334</v>
       </c>
       <c r="K45" s="3" t="n">
-        <v>44068.99739583334</v>
+        <v>44068.93479166667</v>
       </c>
       <c r="L45" s="2" t="n"/>
       <c r="M45" s="2" t="n"/>
       <c r="N45" s="2" t="n"/>
       <c r="O45" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P45" s="2" t="n"/>
       <c r="Q45" s="2" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
@@ -2850,29 +2851,33 @@
       </c>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>Notebook  Asus 636-512</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>ZZZZZ6</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H46" s="3" t="n">
-        <v>44066.73674768519</v>
-      </c>
-      <c r="I46" s="2" t="n"/>
-      <c r="J46" s="2" t="n"/>
-      <c r="K46" s="2" t="n"/>
+        <v>44067.96421296296</v>
+      </c>
+      <c r="I46" s="3" t="n">
+        <v>44068.99569444444</v>
+      </c>
+      <c r="J46" s="3" t="n">
+        <v>44068.77083333334</v>
+      </c>
+      <c r="K46" s="3" t="n">
+        <v>44068.99739583334</v>
+      </c>
       <c r="L46" s="2" t="n"/>
-      <c r="M46" s="3" t="n">
-        <v>44066.78075231481</v>
-      </c>
+      <c r="M46" s="2" t="n"/>
       <c r="N46" s="2" t="n"/>
       <c r="O46" s="2" t="n">
         <v>0</v>
@@ -2885,7 +2890,7 @@
         <v>79</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
@@ -2909,23 +2914,19 @@
       </c>
       <c r="G47" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H47" s="3" t="n">
         <v>44066.73674768519</v>
       </c>
-      <c r="I47" s="3" t="n">
-        <v>44069</v>
-      </c>
-      <c r="J47" s="3" t="n">
-        <v>44069.77083333334</v>
-      </c>
-      <c r="K47" s="3" t="n">
-        <v>44069.00579861111</v>
-      </c>
+      <c r="I47" s="2" t="n"/>
+      <c r="J47" s="2" t="n"/>
+      <c r="K47" s="2" t="n"/>
       <c r="L47" s="2" t="n"/>
-      <c r="M47" s="2" t="n"/>
+      <c r="M47" s="3" t="n">
+        <v>44066.78075231481</v>
+      </c>
       <c r="N47" s="2" t="n"/>
       <c r="O47" s="2" t="n">
         <v>0</v>
@@ -2938,7 +2939,7 @@
         <v>79</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
@@ -2969,13 +2970,13 @@
         <v>44066.73674768519</v>
       </c>
       <c r="I48" s="3" t="n">
-        <v>44068.00912037037</v>
+        <v>44069</v>
       </c>
       <c r="J48" s="3" t="n">
-        <v>44075.77083333334</v>
+        <v>44069.77083333334</v>
       </c>
       <c r="K48" s="3" t="n">
-        <v>44068.94960648148</v>
+        <v>44069.00579861111</v>
       </c>
       <c r="L48" s="2" t="n"/>
       <c r="M48" s="2" t="n"/>
@@ -2988,10 +2989,10 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
@@ -3005,32 +3006,34 @@
       </c>
       <c r="E49" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Notebook  Asus 636-512</t>
         </is>
       </c>
       <c r="F49" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>ZZZZZ6</t>
         </is>
       </c>
       <c r="G49" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H49" s="3" t="n">
-        <v>44064.54511574074</v>
-      </c>
-      <c r="I49" s="2" t="n"/>
-      <c r="J49" s="2" t="n"/>
-      <c r="K49" s="2" t="n"/>
-      <c r="L49" s="3" t="n">
-        <v>44072.77083333334</v>
-      </c>
+        <v>44066.73674768519</v>
+      </c>
+      <c r="I49" s="3" t="n">
+        <v>44068.00912037037</v>
+      </c>
+      <c r="J49" s="3" t="n">
+        <v>44075.77083333334</v>
+      </c>
+      <c r="K49" s="3" t="n">
+        <v>44068.94960648148</v>
+      </c>
+      <c r="L49" s="2" t="n"/>
       <c r="M49" s="2" t="n"/>
-      <c r="N49" s="3" t="n">
-        <v>44064.58971064815</v>
-      </c>
+      <c r="N49" s="2" t="n"/>
       <c r="O49" s="2" t="n">
         <v>0</v>
       </c>
@@ -3042,7 +3045,7 @@
         <v>77</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
@@ -3066,7 +3069,7 @@
       </c>
       <c r="G50" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H50" s="3" t="n">
@@ -3075,11 +3078,13 @@
       <c r="I50" s="2" t="n"/>
       <c r="J50" s="2" t="n"/>
       <c r="K50" s="2" t="n"/>
-      <c r="L50" s="2" t="n"/>
-      <c r="M50" s="3" t="n">
-        <v>44064.58886574074</v>
-      </c>
-      <c r="N50" s="2" t="n"/>
+      <c r="L50" s="3" t="n">
+        <v>44072.77083333334</v>
+      </c>
+      <c r="M50" s="2" t="n"/>
+      <c r="N50" s="3" t="n">
+        <v>44064.58971064815</v>
+      </c>
       <c r="O50" s="2" t="n">
         <v>0</v>
       </c>
@@ -3088,50 +3093,46 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E51" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F51" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H51" s="3" t="n">
-        <v>44062.72828703704</v>
-      </c>
-      <c r="I51" s="3" t="n">
-        <v>44063.58475694444</v>
-      </c>
-      <c r="J51" s="3" t="n">
-        <v>44063.77083333334</v>
-      </c>
-      <c r="K51" s="3" t="n">
-        <v>44063.59297453704</v>
-      </c>
+        <v>44064.54511574074</v>
+      </c>
+      <c r="I51" s="2" t="n"/>
+      <c r="J51" s="2" t="n"/>
+      <c r="K51" s="2" t="n"/>
       <c r="L51" s="2" t="n"/>
-      <c r="M51" s="2" t="n"/>
+      <c r="M51" s="3" t="n">
+        <v>44064.58886574074</v>
+      </c>
       <c r="N51" s="2" t="n"/>
       <c r="O51" s="2" t="n">
         <v>0</v>
@@ -3141,19 +3142,19 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D52" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E52" s="2" t="inlineStr">
@@ -3172,32 +3173,32 @@
         </is>
       </c>
       <c r="H52" s="3" t="n">
-        <v>44059.52234953704</v>
+        <v>44062.72828703704</v>
       </c>
       <c r="I52" s="3" t="n">
-        <v>44059.5640162037</v>
+        <v>44063.58475694444</v>
       </c>
       <c r="J52" s="3" t="n">
-        <v>44077.77083333334</v>
+        <v>44063.77083333334</v>
       </c>
       <c r="K52" s="3" t="n">
-        <v>44064.57136574074</v>
+        <v>44063.59297453704</v>
       </c>
       <c r="L52" s="2" t="n"/>
       <c r="M52" s="2" t="n"/>
       <c r="N52" s="2" t="n"/>
       <c r="O52" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P52" s="2" t="n"/>
       <c r="Q52" s="2" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
@@ -3211,12 +3212,12 @@
       </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F53" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G53" s="2" t="inlineStr">
@@ -3225,32 +3226,32 @@
         </is>
       </c>
       <c r="H53" s="3" t="n">
-        <v>44059.4880787037</v>
+        <v>44059.52234953704</v>
       </c>
       <c r="I53" s="3" t="n">
-        <v>44059.53171296296</v>
+        <v>44059.5640162037</v>
       </c>
       <c r="J53" s="3" t="n">
-        <v>44071.77083333334</v>
+        <v>44077.77083333334</v>
       </c>
       <c r="K53" s="3" t="n">
-        <v>44070.67811342593</v>
+        <v>44064.57136574074</v>
       </c>
       <c r="L53" s="2" t="n"/>
       <c r="M53" s="2" t="n"/>
       <c r="N53" s="2" t="n"/>
       <c r="O53" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P53" s="2" t="n"/>
       <c r="Q53" s="2" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
@@ -3264,12 +3265,12 @@
       </c>
       <c r="E54" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G54" s="2" t="inlineStr">
@@ -3278,16 +3279,16 @@
         </is>
       </c>
       <c r="H54" s="3" t="n">
-        <v>44058.48174768518</v>
+        <v>44059.4880787037</v>
       </c>
       <c r="I54" s="3" t="n">
-        <v>44059.53150462963</v>
+        <v>44059.53171296296</v>
       </c>
       <c r="J54" s="3" t="n">
-        <v>44061.77083333334</v>
+        <v>44071.77083333334</v>
       </c>
       <c r="K54" s="3" t="n">
-        <v>44062.5589699074</v>
+        <v>44070.67811342593</v>
       </c>
       <c r="L54" s="2" t="n"/>
       <c r="M54" s="2" t="n"/>
@@ -3300,19 +3301,19 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E55" s="2" t="inlineStr">
@@ -3327,18 +3328,22 @@
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H55" s="3" t="n">
-        <v>44053.7452662037</v>
-      </c>
-      <c r="I55" s="2" t="n"/>
-      <c r="J55" s="2" t="n"/>
-      <c r="K55" s="2" t="n"/>
-      <c r="L55" s="3" t="n">
+        <v>44058.48174768518</v>
+      </c>
+      <c r="I55" s="3" t="n">
+        <v>44059.53150462963</v>
+      </c>
+      <c r="J55" s="3" t="n">
         <v>44061.77083333334</v>
       </c>
+      <c r="K55" s="3" t="n">
+        <v>44062.5589699074</v>
+      </c>
+      <c r="L55" s="2" t="n"/>
       <c r="M55" s="2" t="n"/>
       <c r="N55" s="2" t="n"/>
       <c r="O55" s="2" t="n">
@@ -3349,82 +3354,78 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>198182354</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
         <is>
-          <t>Víctor Esteban Sánchez Ulloa</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E56" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G56" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H56" s="3" t="n">
-        <v>44051.89761574074</v>
-      </c>
-      <c r="I56" s="3" t="n">
-        <v>44051.94155092593</v>
-      </c>
-      <c r="J56" s="3" t="n">
-        <v>44155.77083333334</v>
-      </c>
-      <c r="K56" s="3" t="n">
-        <v>44110.99850694444</v>
-      </c>
-      <c r="L56" s="2" t="n"/>
+        <v>44053.7452662037</v>
+      </c>
+      <c r="I56" s="2" t="n"/>
+      <c r="J56" s="2" t="n"/>
+      <c r="K56" s="2" t="n"/>
+      <c r="L56" s="3" t="n">
+        <v>44061.77083333334</v>
+      </c>
       <c r="M56" s="2" t="n"/>
       <c r="N56" s="2" t="n"/>
       <c r="O56" s="2" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="P56" s="2" t="n"/>
       <c r="Q56" s="2" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>19988806K</t>
+          <t>198182354</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Toro</t>
+          <t>Víctor Esteban Sánchez Ulloa</t>
         </is>
       </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F57" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G57" s="2" t="inlineStr">
@@ -3433,64 +3434,70 @@
         </is>
       </c>
       <c r="H57" s="3" t="n">
-        <v>44051.60150462963</v>
+        <v>44051.89761574074</v>
       </c>
       <c r="I57" s="3" t="n">
-        <v>44051.6865625</v>
+        <v>44051.94155092593</v>
       </c>
       <c r="J57" s="3" t="n">
-        <v>44053.77083333334</v>
+        <v>44155.77083333334</v>
       </c>
       <c r="K57" s="3" t="n">
-        <v>44053.79626157408</v>
+        <v>44110.99850694444</v>
       </c>
       <c r="L57" s="2" t="n"/>
       <c r="M57" s="2" t="n"/>
       <c r="N57" s="2" t="n"/>
       <c r="O57" s="2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P57" s="2" t="n"/>
       <c r="Q57" s="2" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Drone Parrot Bebop 2</t>
         </is>
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>ABC432</t>
         </is>
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H58" s="3" t="n">
-        <v>44050.4183449074</v>
-      </c>
-      <c r="I58" s="2" t="n"/>
-      <c r="J58" s="2" t="n"/>
-      <c r="K58" s="2" t="n"/>
+        <v>44051.60150462963</v>
+      </c>
+      <c r="I58" s="3" t="n">
+        <v>44051.6865625</v>
+      </c>
+      <c r="J58" s="3" t="n">
+        <v>44053.77083333334</v>
+      </c>
+      <c r="K58" s="3" t="n">
+        <v>44053.79626157408</v>
+      </c>
       <c r="L58" s="2" t="n"/>
       <c r="M58" s="2" t="n"/>
       <c r="N58" s="2" t="n"/>
@@ -3505,7 +3512,7 @@
         <v>63</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
@@ -3519,12 +3526,12 @@
       </c>
       <c r="E59" s="2" t="inlineStr">
         <is>
-          <t>Celular Samsung Galaxy S4</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F59" s="2" t="inlineStr">
         <is>
-          <t>AAD832</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G59" s="2" t="inlineStr">
@@ -3552,7 +3559,7 @@
         <v>63</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
@@ -3576,21 +3583,15 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H60" s="3" t="n">
         <v>44050.4183449074</v>
       </c>
-      <c r="I60" s="3" t="n">
-        <v>44051.54168981482</v>
-      </c>
-      <c r="J60" s="3" t="n">
-        <v>44051.77083333334</v>
-      </c>
-      <c r="K60" s="3" t="n">
-        <v>44051.54444444444</v>
-      </c>
+      <c r="I60" s="2" t="n"/>
+      <c r="J60" s="2" t="n"/>
+      <c r="K60" s="2" t="n"/>
       <c r="L60" s="2" t="n"/>
       <c r="M60" s="2" t="n"/>
       <c r="N60" s="2" t="n"/>
@@ -3602,10 +3603,10 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
@@ -3619,28 +3620,32 @@
       </c>
       <c r="E61" s="2" t="inlineStr">
         <is>
-          <t>Placa Raspberry Raspberry Pi B+</t>
+          <t>Celular Samsung Galaxy S4</t>
         </is>
       </c>
       <c r="F61" s="2" t="inlineStr">
         <is>
-          <t>AAA192</t>
+          <t>AAD832</t>
         </is>
       </c>
       <c r="G61" s="2" t="inlineStr">
         <is>
-          <t>Cancelada</t>
+          <t>Finalizada</t>
         </is>
       </c>
       <c r="H61" s="3" t="n">
-        <v>44047.52844907407</v>
-      </c>
-      <c r="I61" s="2" t="n"/>
-      <c r="J61" s="2" t="n"/>
-      <c r="K61" s="2" t="n"/>
-      <c r="L61" s="3" t="n">
-        <v>44049.77083333334</v>
-      </c>
+        <v>44050.4183449074</v>
+      </c>
+      <c r="I61" s="3" t="n">
+        <v>44051.54168981482</v>
+      </c>
+      <c r="J61" s="3" t="n">
+        <v>44051.77083333334</v>
+      </c>
+      <c r="K61" s="3" t="n">
+        <v>44051.54444444444</v>
+      </c>
+      <c r="L61" s="2" t="n"/>
       <c r="M61" s="2" t="n"/>
       <c r="N61" s="2" t="n"/>
       <c r="O61" s="2" t="n">
@@ -3651,10 +3656,10 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
@@ -3668,26 +3673,28 @@
       </c>
       <c r="E62" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Placa Raspberry Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>AAA192</t>
         </is>
       </c>
       <c r="G62" s="2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Cancelada</t>
         </is>
       </c>
       <c r="H62" s="3" t="n">
-        <v>44047.49662037037</v>
+        <v>44047.52844907407</v>
       </c>
       <c r="I62" s="2" t="n"/>
       <c r="J62" s="2" t="n"/>
       <c r="K62" s="2" t="n"/>
-      <c r="L62" s="2" t="n"/>
+      <c r="L62" s="3" t="n">
+        <v>44049.77083333334</v>
+      </c>
       <c r="M62" s="2" t="n"/>
       <c r="N62" s="2" t="n"/>
       <c r="O62" s="2" t="n">
@@ -3698,48 +3705,42 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
-          <t>198182354</t>
+          <t>19889608K</t>
         </is>
       </c>
       <c r="D63" s="2" t="inlineStr">
         <is>
-          <t>Víctor Esteban Sánchez Ulloa</t>
+          <t>Sebastián Ignacio Toro Severino</t>
         </is>
       </c>
       <c r="E63" s="2" t="inlineStr">
         <is>
-          <t>Router TP-LINK TL-WN722N</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F63" s="2" t="inlineStr">
         <is>
-          <t>AAA351</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G63" s="2" t="inlineStr">
         <is>
-          <t>Finalizada</t>
+          <t>Rechazada</t>
         </is>
       </c>
       <c r="H63" s="3" t="n">
-        <v>44045.12303240741</v>
-      </c>
-      <c r="I63" s="3" t="n">
-        <v>44048.15038194445</v>
-      </c>
-      <c r="J63" s="3" t="n">
-        <v>44060.77083333334</v>
-      </c>
-      <c r="K63" s="3" t="n">
-        <v>44048.15122685185</v>
-      </c>
+        <v>44047.49662037037</v>
+      </c>
+      <c r="I63" s="2" t="n"/>
+      <c r="J63" s="2" t="n"/>
+      <c r="K63" s="2" t="n"/>
       <c r="L63" s="2" t="n"/>
       <c r="M63" s="2" t="n"/>
       <c r="N63" s="2" t="n"/>
@@ -3751,19 +3752,19 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>19889608K</t>
+          <t>198182354</t>
         </is>
       </c>
       <c r="D64" s="2" t="inlineStr">
         <is>
-          <t>Sebastián Ignacio Toro Severino</t>
+          <t>Víctor Esteban Sánchez Ulloa</t>
         </is>
       </c>
       <c r="E64" s="2" t="inlineStr">
@@ -3782,16 +3783,16 @@
         </is>
       </c>
       <c r="H64" s="3" t="n">
-        <v>44044.55893518519</v>
+        <v>44045.12303240741</v>
       </c>
       <c r="I64" s="3" t="n">
-        <v>44044.60060185185</v>
+        <v>44048.15038194445</v>
       </c>
       <c r="J64" s="3" t="n">
-        <v>44050.77083333334</v>
+        <v>44060.77083333334</v>
       </c>
       <c r="K64" s="3" t="n">
-        <v>44050.4495949074</v>
+        <v>44048.15122685185</v>
       </c>
       <c r="L64" s="2" t="n"/>
       <c r="M64" s="2" t="n"/>
@@ -3804,10 +3805,10 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
@@ -3821,12 +3822,12 @@
       </c>
       <c r="E65" s="2" t="inlineStr">
         <is>
-          <t>Disco duro Toshiba Canvio 2 TB</t>
+          <t>Router TP-LINK TL-WN722N</t>
         </is>
       </c>
       <c r="F65" s="2" t="inlineStr">
         <is>
-          <t>AA431</t>
+          <t>AAA351</t>
         </is>
       </c>
       <c r="G65" s="2" t="inlineStr">
@@ -3835,16 +3836,16 @@
         </is>
       </c>
       <c r="H65" s="3" t="n">
-        <v>44044.53820601852</v>
+        <v>44044.55893518519</v>
       </c>
       <c r="I65" s="3" t="n">
-        <v>44044.57987268519</v>
+        <v>44044.60060185185</v>
       </c>
       <c r="J65" s="3" t="n">
-        <v>44056.77083333334</v>
+        <v>44050.77083333334</v>
       </c>
       <c r="K65" s="3" t="n">
-        <v>44059.50581018518</v>
+        <v>44050.4495949074</v>
       </c>
       <c r="L65" s="2" t="n"/>
       <c r="M65" s="2" t="n"/>
@@ -3860,7 +3861,7 @@
         <v>48</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
@@ -3874,12 +3875,12 @@
       </c>
       <c r="E66" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Disco duro Toshiba Canvio 2 TB</t>
         </is>
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>AA431</t>
         </is>
       </c>
       <c r="G66" s="2" t="inlineStr">
@@ -3894,10 +3895,10 @@
         <v>44044.57987268519</v>
       </c>
       <c r="J66" s="3" t="n">
-        <v>44048.77083333334</v>
+        <v>44056.77083333334</v>
       </c>
       <c r="K66" s="3" t="n">
-        <v>44049.66491898148</v>
+        <v>44059.50581018518</v>
       </c>
       <c r="L66" s="2" t="n"/>
       <c r="M66" s="2" t="n"/>
@@ -3913,7 +3914,7 @@
         <v>47</v>
       </c>
       <c r="B67" s="2" t="n">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
@@ -3960,7 +3961,7 @@
         <v>47</v>
       </c>
       <c r="B68" s="2" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
@@ -4007,7 +4008,7 @@
         <v>47</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>

</xml_diff>